<commit_message>
Matriz de Pruebas Auditorias
</commit_message>
<xml_diff>
--- a/PABMI/ENTREGABLES/Matriz de Pruebas Configuraciones Catálogos BIENES MUEBLES.xlsx
+++ b/PABMI/ENTREGABLES/Matriz de Pruebas Configuraciones Catálogos BIENES MUEBLES.xlsx
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="133">
   <si>
     <t>Matriz de Pruebas Plataforma de Administración de Bienes Muebles e Inmuebles</t>
   </si>
@@ -488,9 +488,6 @@
     <t xml:space="preserve">Arroja un error al ingresar al menú no permite realizar otra función </t>
   </si>
   <si>
-    <t>https://pabmi.atlassian.net/browse/PABMI-813</t>
-  </si>
-  <si>
     <t>https://pabmi.atlassian.net/browse/PABMI-814</t>
   </si>
   <si>
@@ -513,6 +510,12 @@
   </si>
   <si>
     <t>https://pabmi.atlassian.net/browse/PABMI-817</t>
+  </si>
+  <si>
+    <t>https://pabmi.atlassian.net/browse/PABMI-804</t>
+  </si>
+  <si>
+    <t>https://pabmi.atlassian.net/browse/PABMI-813    https://pabmi.atlassian.net/browse/PABMI-915</t>
   </si>
 </sst>
 </file>
@@ -869,6 +872,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -919,39 +955,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1107,7 +1110,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1601,9 +1603,7 @@
           <c:showPercent val="1"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -1667,9 +1667,7 @@
           <c:showPercent val="1"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -1733,9 +1731,7 @@
           <c:showPercent val="1"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -1856,9 +1852,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000021-296A-4B28-822E-076088C40B78}"/>
                 </c:ext>
@@ -1879,9 +1873,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000001F-296A-4B28-822E-076088C40B78}"/>
                 </c:ext>
@@ -2138,7 +2130,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2527,7 +2518,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2648,7 +2638,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3598,7 +3587,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7536,7 +7524,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
   <location ref="A24:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField dataField="1" showAll="0"/>
@@ -7601,7 +7589,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -7708,7 +7696,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A47:D50" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -8061,10 +8049,10 @@
   <dimension ref="A1:N117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="9" topLeftCell="H48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I79" sqref="I79"/>
+      <selection pane="bottomRight" activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8085,94 +8073,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="28" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="33" t="s">
+      <c r="B5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
@@ -8320,7 +8308,7 @@
       <c r="M9" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="N9" s="48">
+      <c r="N9" s="21">
         <v>45114</v>
       </c>
     </row>
@@ -8362,7 +8350,7 @@
       <c r="M10" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="N10" s="48">
+      <c r="N10" s="21">
         <v>45114</v>
       </c>
     </row>
@@ -8404,7 +8392,7 @@
       <c r="M11" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="N11" s="48">
+      <c r="N11" s="21">
         <v>45114</v>
       </c>
     </row>
@@ -8437,22 +8425,22 @@
         <v>77</v>
       </c>
       <c r="J12" s="2"/>
-      <c r="N12" s="48"/>
+      <c r="N12" s="21"/>
     </row>
     <row r="13" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="38">
+      <c r="A13" s="26">
         <v>7</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="E13" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F13" s="3" t="s">
@@ -8468,19 +8456,19 @@
         <v>92</v>
       </c>
       <c r="J13" s="2"/>
-      <c r="M13" s="45" t="s">
+      <c r="M13" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="N13" s="46">
+      <c r="N13" s="23">
         <v>45142</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
       <c r="F14" s="3" t="s">
         <v>32</v>
       </c>
@@ -8492,15 +8480,15 @@
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="2"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="46"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="23"/>
     </row>
     <row r="15" spans="1:14" ht="33" x14ac:dyDescent="0.3">
-      <c r="A15" s="38"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
       <c r="F15" s="3" t="s">
         <v>33</v>
       </c>
@@ -8518,17 +8506,17 @@
         <v>74</v>
       </c>
       <c r="L15" t="s">
-        <v>57</v>
-      </c>
-      <c r="M15" s="43"/>
-      <c r="N15" s="46"/>
+        <v>58</v>
+      </c>
+      <c r="M15" s="24"/>
+      <c r="N15" s="23"/>
     </row>
     <row r="16" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="38"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
       <c r="F16" s="3" t="s">
         <v>34</v>
       </c>
@@ -8546,17 +8534,17 @@
         <v>74</v>
       </c>
       <c r="L16" t="s">
-        <v>57</v>
-      </c>
-      <c r="M16" s="43"/>
-      <c r="N16" s="46"/>
+        <v>58</v>
+      </c>
+      <c r="M16" s="24"/>
+      <c r="N16" s="23"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="38"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
       <c r="F17" s="3" t="s">
         <v>35</v>
       </c>
@@ -8570,15 +8558,15 @@
         <v>98</v>
       </c>
       <c r="J17" s="2"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="46"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="23"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="38"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
       <c r="F18" s="3" t="s">
         <v>36</v>
       </c>
@@ -8596,17 +8584,17 @@
         <v>74</v>
       </c>
       <c r="L18" t="s">
-        <v>57</v>
-      </c>
-      <c r="M18" s="43"/>
-      <c r="N18" s="46"/>
+        <v>58</v>
+      </c>
+      <c r="M18" s="24"/>
+      <c r="N18" s="23"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="38"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
       <c r="F19" s="3" t="s">
         <v>37</v>
       </c>
@@ -8620,23 +8608,23 @@
         <v>104</v>
       </c>
       <c r="J19" s="2"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="46"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="23"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="38">
+      <c r="A20" s="26">
         <v>8</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -8655,21 +8643,21 @@
         <v>74</v>
       </c>
       <c r="L20" t="s">
-        <v>57</v>
-      </c>
-      <c r="M20" s="44" t="s">
-        <v>127</v>
-      </c>
-      <c r="N20" s="47">
+        <v>58</v>
+      </c>
+      <c r="M20" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="N20" s="31">
         <v>45145</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="38"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
       <c r="F21" s="3" t="s">
         <v>32</v>
       </c>
@@ -8686,17 +8674,17 @@
         <v>74</v>
       </c>
       <c r="L21" t="s">
-        <v>57</v>
-      </c>
-      <c r="M21" s="42"/>
-      <c r="N21" s="47"/>
+        <v>58</v>
+      </c>
+      <c r="M21" s="30"/>
+      <c r="N21" s="31"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="38"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
       <c r="F22" s="3" t="s">
         <v>33</v>
       </c>
@@ -8713,17 +8701,17 @@
         <v>74</v>
       </c>
       <c r="L22" t="s">
-        <v>57</v>
-      </c>
-      <c r="M22" s="42"/>
-      <c r="N22" s="47"/>
+        <v>58</v>
+      </c>
+      <c r="M22" s="30"/>
+      <c r="N22" s="31"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="38"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
       <c r="F23" s="3" t="s">
         <v>34</v>
       </c>
@@ -8740,17 +8728,17 @@
         <v>74</v>
       </c>
       <c r="L23" t="s">
-        <v>57</v>
-      </c>
-      <c r="M23" s="42"/>
-      <c r="N23" s="47"/>
+        <v>58</v>
+      </c>
+      <c r="M23" s="30"/>
+      <c r="N23" s="31"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="38"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
       <c r="F24" s="3" t="s">
         <v>35</v>
       </c>
@@ -8763,15 +8751,15 @@
       <c r="I24" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="M24" s="42"/>
-      <c r="N24" s="47"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="31"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="38"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
       <c r="F25" s="3" t="s">
         <v>36</v>
       </c>
@@ -8788,17 +8776,17 @@
         <v>74</v>
       </c>
       <c r="L25" t="s">
-        <v>57</v>
-      </c>
-      <c r="M25" s="42"/>
-      <c r="N25" s="47"/>
+        <v>58</v>
+      </c>
+      <c r="M25" s="30"/>
+      <c r="N25" s="31"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="38"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
       <c r="F26" s="3" t="s">
         <v>37</v>
       </c>
@@ -8811,23 +8799,23 @@
       <c r="I26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="M26" s="42"/>
-      <c r="N26" s="47"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="31"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="38">
+      <c r="A27" s="26">
         <v>9</v>
       </c>
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="40" t="s">
+      <c r="C27" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="41" t="s">
+      <c r="D27" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="41" t="s">
+      <c r="E27" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F27" s="3" t="s">
@@ -8848,19 +8836,19 @@
       <c r="L27" t="s">
         <v>57</v>
       </c>
-      <c r="M27" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="N27" s="47">
+      <c r="M27" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="N27" s="31">
         <v>45145</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="38"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
       <c r="F28" s="3" t="s">
         <v>32</v>
       </c>
@@ -8879,15 +8867,15 @@
       <c r="L28" t="s">
         <v>57</v>
       </c>
-      <c r="M28" s="45"/>
-      <c r="N28" s="47"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="31"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" s="38"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
       <c r="F29" s="3" t="s">
         <v>33</v>
       </c>
@@ -8906,15 +8894,15 @@
       <c r="L29" t="s">
         <v>57</v>
       </c>
-      <c r="M29" s="45"/>
-      <c r="N29" s="47"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="31"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="38"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
       <c r="F30" s="3" t="s">
         <v>34</v>
       </c>
@@ -8933,15 +8921,15 @@
       <c r="L30" t="s">
         <v>57</v>
       </c>
-      <c r="M30" s="45"/>
-      <c r="N30" s="47"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="31"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="38"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
       <c r="F31" s="3" t="s">
         <v>35</v>
       </c>
@@ -8954,15 +8942,15 @@
       <c r="I31" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="M31" s="45"/>
-      <c r="N31" s="47"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="31"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" s="38"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
       <c r="F32" s="3" t="s">
         <v>36</v>
       </c>
@@ -8981,15 +8969,15 @@
       <c r="L32" t="s">
         <v>57</v>
       </c>
-      <c r="M32" s="45"/>
-      <c r="N32" s="47"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="31"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="38"/>
-      <c r="B33" s="39"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
       <c r="F33" s="3" t="s">
         <v>37</v>
       </c>
@@ -9002,23 +8990,23 @@
       <c r="I33" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="M33" s="45"/>
-      <c r="N33" s="47"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="31"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="38">
+      <c r="A34" s="26">
         <v>10</v>
       </c>
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="41" t="s">
+      <c r="D34" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E34" s="41" t="s">
+      <c r="E34" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F34" s="3" t="s">
@@ -9039,19 +9027,19 @@
       <c r="L34" t="s">
         <v>57</v>
       </c>
-      <c r="M34" s="44" t="s">
-        <v>128</v>
-      </c>
-      <c r="N34" s="47">
+      <c r="M34" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="N34" s="31">
         <v>45145</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="38"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
       <c r="F35" s="3" t="s">
         <v>32</v>
       </c>
@@ -9070,15 +9058,15 @@
       <c r="L35" t="s">
         <v>57</v>
       </c>
-      <c r="M35" s="42"/>
-      <c r="N35" s="47"/>
+      <c r="M35" s="30"/>
+      <c r="N35" s="31"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="38"/>
-      <c r="B36" s="39"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
       <c r="F36" s="3" t="s">
         <v>33</v>
       </c>
@@ -9097,15 +9085,15 @@
       <c r="L36" t="s">
         <v>57</v>
       </c>
-      <c r="M36" s="42"/>
-      <c r="N36" s="47"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="31"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="38"/>
-      <c r="B37" s="39"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
       <c r="F37" s="3" t="s">
         <v>34</v>
       </c>
@@ -9124,15 +9112,15 @@
       <c r="L37" t="s">
         <v>57</v>
       </c>
-      <c r="M37" s="42"/>
-      <c r="N37" s="47"/>
+      <c r="M37" s="30"/>
+      <c r="N37" s="31"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="38"/>
-      <c r="B38" s="39"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
       <c r="F38" s="3" t="s">
         <v>35</v>
       </c>
@@ -9145,15 +9133,15 @@
       <c r="I38" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="M38" s="42"/>
-      <c r="N38" s="47"/>
+      <c r="M38" s="30"/>
+      <c r="N38" s="31"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="38"/>
-      <c r="B39" s="39"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
       <c r="F39" s="3" t="s">
         <v>36</v>
       </c>
@@ -9172,15 +9160,15 @@
       <c r="L39" t="s">
         <v>57</v>
       </c>
-      <c r="M39" s="42"/>
-      <c r="N39" s="47"/>
+      <c r="M39" s="30"/>
+      <c r="N39" s="31"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="38"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
       <c r="F40" s="3" t="s">
         <v>37</v>
       </c>
@@ -9193,23 +9181,23 @@
       <c r="I40" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="M40" s="42"/>
-      <c r="N40" s="47"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="31"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" s="38">
+      <c r="A41" s="26">
         <v>11</v>
       </c>
-      <c r="B41" s="39" t="s">
+      <c r="B41" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="40" t="s">
+      <c r="C41" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="D41" s="41" t="s">
+      <c r="D41" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E41" s="41" t="s">
+      <c r="E41" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F41" s="3" t="s">
@@ -9224,19 +9212,19 @@
       <c r="I41" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="M41" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="N41" s="46">
+      <c r="M41" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="N41" s="23">
         <v>45142</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="66" x14ac:dyDescent="0.3">
-      <c r="A42" s="38"/>
-      <c r="B42" s="39"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="41"/>
-      <c r="E42" s="41"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
       <c r="F42" s="3" t="s">
         <v>32</v>
       </c>
@@ -9253,17 +9241,17 @@
         <v>74</v>
       </c>
       <c r="L42" t="s">
-        <v>57</v>
-      </c>
-      <c r="M42" s="45"/>
-      <c r="N42" s="46"/>
+        <v>58</v>
+      </c>
+      <c r="M42" s="22"/>
+      <c r="N42" s="23"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" s="38"/>
-      <c r="B43" s="39"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
       <c r="F43" s="3" t="s">
         <v>33</v>
       </c>
@@ -9280,17 +9268,17 @@
         <v>74</v>
       </c>
       <c r="L43" t="s">
-        <v>57</v>
-      </c>
-      <c r="M43" s="45"/>
-      <c r="N43" s="46"/>
+        <v>58</v>
+      </c>
+      <c r="M43" s="22"/>
+      <c r="N43" s="23"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A44" s="38"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
       <c r="F44" s="3" t="s">
         <v>34</v>
       </c>
@@ -9307,17 +9295,17 @@
         <v>74</v>
       </c>
       <c r="L44" t="s">
-        <v>57</v>
-      </c>
-      <c r="M44" s="45"/>
-      <c r="N44" s="46"/>
+        <v>58</v>
+      </c>
+      <c r="M44" s="22"/>
+      <c r="N44" s="23"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A45" s="38"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="41"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
       <c r="F45" s="3" t="s">
         <v>35</v>
       </c>
@@ -9330,15 +9318,15 @@
       <c r="I45" t="s">
         <v>98</v>
       </c>
-      <c r="M45" s="45"/>
-      <c r="N45" s="46"/>
+      <c r="M45" s="22"/>
+      <c r="N45" s="23"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A46" s="38"/>
-      <c r="B46" s="39"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
       <c r="F46" s="3" t="s">
         <v>36</v>
       </c>
@@ -9355,17 +9343,17 @@
         <v>74</v>
       </c>
       <c r="L46" t="s">
-        <v>57</v>
-      </c>
-      <c r="M46" s="45"/>
-      <c r="N46" s="46"/>
+        <v>58</v>
+      </c>
+      <c r="M46" s="22"/>
+      <c r="N46" s="23"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A47" s="38"/>
-      <c r="B47" s="39"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
       <c r="F47" s="3" t="s">
         <v>37</v>
       </c>
@@ -9378,23 +9366,23 @@
       <c r="I47" t="s">
         <v>104</v>
       </c>
-      <c r="M47" s="45"/>
-      <c r="N47" s="46"/>
+      <c r="M47" s="22"/>
+      <c r="N47" s="23"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A48" s="38">
+      <c r="A48" s="26">
         <v>12</v>
       </c>
-      <c r="B48" s="39" t="s">
+      <c r="B48" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="40" t="s">
+      <c r="C48" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D48" s="41" t="s">
+      <c r="D48" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E48" s="41" t="s">
+      <c r="E48" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F48" s="3" t="s">
@@ -9413,26 +9401,26 @@
         <v>74</v>
       </c>
       <c r="L48" t="s">
-        <v>57</v>
-      </c>
-      <c r="M48" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="N48" s="47">
+        <v>58</v>
+      </c>
+      <c r="M48" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="N48" s="31">
         <v>45145</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A49" s="38"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="40"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
       <c r="F49" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G49" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H49" t="s">
         <v>118</v>
@@ -9444,22 +9432,22 @@
         <v>74</v>
       </c>
       <c r="L49" t="s">
-        <v>57</v>
-      </c>
-      <c r="M49" s="43"/>
-      <c r="N49" s="47"/>
+        <v>58</v>
+      </c>
+      <c r="M49" s="24"/>
+      <c r="N49" s="31"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A50" s="38"/>
-      <c r="B50" s="39"/>
-      <c r="C50" s="40"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="41"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
       <c r="F50" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G50" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H50" t="s">
         <v>117</v>
@@ -9471,22 +9459,22 @@
         <v>74</v>
       </c>
       <c r="L50" t="s">
-        <v>57</v>
-      </c>
-      <c r="M50" s="43"/>
-      <c r="N50" s="47"/>
+        <v>58</v>
+      </c>
+      <c r="M50" s="24"/>
+      <c r="N50" s="31"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A51" s="38"/>
-      <c r="B51" s="39"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="41"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
       <c r="F51" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G51" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H51" t="s">
         <v>117</v>
@@ -9498,17 +9486,17 @@
         <v>74</v>
       </c>
       <c r="L51" t="s">
-        <v>57</v>
-      </c>
-      <c r="M51" s="43"/>
-      <c r="N51" s="47"/>
+        <v>58</v>
+      </c>
+      <c r="M51" s="24"/>
+      <c r="N51" s="31"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A52" s="38"/>
-      <c r="B52" s="39"/>
-      <c r="C52" s="40"/>
-      <c r="D52" s="41"/>
-      <c r="E52" s="41"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
       <c r="F52" s="3" t="s">
         <v>35</v>
       </c>
@@ -9521,15 +9509,15 @@
       <c r="I52" t="s">
         <v>98</v>
       </c>
-      <c r="M52" s="43"/>
-      <c r="N52" s="47"/>
+      <c r="M52" s="24"/>
+      <c r="N52" s="31"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A53" s="38"/>
-      <c r="B53" s="39"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="41"/>
-      <c r="E53" s="41"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
       <c r="F53" s="3" t="s">
         <v>36</v>
       </c>
@@ -9546,17 +9534,17 @@
         <v>74</v>
       </c>
       <c r="L53" t="s">
-        <v>57</v>
-      </c>
-      <c r="M53" s="43"/>
-      <c r="N53" s="47"/>
+        <v>62</v>
+      </c>
+      <c r="M53" s="24"/>
+      <c r="N53" s="31"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A54" s="38"/>
-      <c r="B54" s="39"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="41"/>
-      <c r="E54" s="41"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
       <c r="F54" s="3" t="s">
         <v>37</v>
       </c>
@@ -9569,23 +9557,23 @@
       <c r="I54" t="s">
         <v>104</v>
       </c>
-      <c r="M54" s="43"/>
-      <c r="N54" s="47"/>
+      <c r="M54" s="24"/>
+      <c r="N54" s="31"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A55" s="38">
+      <c r="A55" s="26">
         <v>13</v>
       </c>
-      <c r="B55" s="39" t="s">
+      <c r="B55" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C55" s="40" t="s">
+      <c r="C55" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D55" s="41" t="s">
+      <c r="D55" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E55" s="41" t="s">
+      <c r="E55" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F55" s="3" t="s">
@@ -9604,26 +9592,26 @@
         <v>74</v>
       </c>
       <c r="L55" t="s">
-        <v>57</v>
-      </c>
-      <c r="M55" s="45" t="s">
-        <v>124</v>
-      </c>
-      <c r="N55" s="46">
+        <v>58</v>
+      </c>
+      <c r="M55" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="N55" s="23">
         <v>45145</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A56" s="38"/>
-      <c r="B56" s="39"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="41"/>
-      <c r="E56" s="41"/>
+      <c r="A56" s="26"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
       <c r="F56" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G56" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H56" t="s">
         <v>118</v>
@@ -9635,22 +9623,22 @@
         <v>74</v>
       </c>
       <c r="L56" t="s">
-        <v>57</v>
-      </c>
-      <c r="M56" s="45"/>
-      <c r="N56" s="46"/>
+        <v>58</v>
+      </c>
+      <c r="M56" s="22"/>
+      <c r="N56" s="23"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A57" s="38"/>
-      <c r="B57" s="39"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="41"/>
-      <c r="E57" s="41"/>
+      <c r="A57" s="26"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
       <c r="F57" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G57" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H57" t="s">
         <v>117</v>
@@ -9662,22 +9650,22 @@
         <v>74</v>
       </c>
       <c r="L57" t="s">
-        <v>57</v>
-      </c>
-      <c r="M57" s="45"/>
-      <c r="N57" s="46"/>
+        <v>58</v>
+      </c>
+      <c r="M57" s="22"/>
+      <c r="N57" s="23"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A58" s="38"/>
-      <c r="B58" s="39"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="41"/>
-      <c r="E58" s="41"/>
+      <c r="A58" s="26"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
       <c r="F58" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G58" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H58" t="s">
         <v>117</v>
@@ -9689,17 +9677,17 @@
         <v>74</v>
       </c>
       <c r="L58" t="s">
-        <v>57</v>
-      </c>
-      <c r="M58" s="45"/>
-      <c r="N58" s="46"/>
+        <v>58</v>
+      </c>
+      <c r="M58" s="22"/>
+      <c r="N58" s="23"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A59" s="38"/>
-      <c r="B59" s="39"/>
-      <c r="C59" s="40"/>
-      <c r="D59" s="41"/>
-      <c r="E59" s="41"/>
+      <c r="A59" s="26"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="25"/>
       <c r="F59" s="3" t="s">
         <v>35</v>
       </c>
@@ -9712,15 +9700,15 @@
       <c r="I59" t="s">
         <v>98</v>
       </c>
-      <c r="M59" s="45"/>
-      <c r="N59" s="46"/>
+      <c r="M59" s="22"/>
+      <c r="N59" s="23"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A60" s="38"/>
-      <c r="B60" s="39"/>
-      <c r="C60" s="40"/>
-      <c r="D60" s="41"/>
-      <c r="E60" s="41"/>
+      <c r="A60" s="26"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
       <c r="F60" s="3" t="s">
         <v>36</v>
       </c>
@@ -9739,15 +9727,15 @@
       <c r="L60" t="s">
         <v>57</v>
       </c>
-      <c r="M60" s="45"/>
-      <c r="N60" s="46"/>
+      <c r="M60" s="22"/>
+      <c r="N60" s="23"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A61" s="38"/>
-      <c r="B61" s="39"/>
-      <c r="C61" s="40"/>
-      <c r="D61" s="41"/>
-      <c r="E61" s="41"/>
+      <c r="A61" s="26"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="25"/>
       <c r="F61" s="3" t="s">
         <v>37</v>
       </c>
@@ -9760,23 +9748,23 @@
       <c r="I61" t="s">
         <v>104</v>
       </c>
-      <c r="M61" s="45"/>
-      <c r="N61" s="46"/>
+      <c r="M61" s="22"/>
+      <c r="N61" s="23"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A62" s="38">
+      <c r="A62" s="26">
         <v>14</v>
       </c>
-      <c r="B62" s="39" t="s">
+      <c r="B62" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C62" s="40" t="s">
+      <c r="C62" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D62" s="41" t="s">
+      <c r="D62" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E62" s="41" t="s">
+      <c r="E62" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F62" s="3" t="s">
@@ -9791,19 +9779,19 @@
       <c r="I62" t="s">
         <v>77</v>
       </c>
-      <c r="M62" s="45" t="s">
-        <v>131</v>
-      </c>
-      <c r="N62" s="46">
+      <c r="M62" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="N62" s="23">
         <v>45145</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A63" s="38"/>
-      <c r="B63" s="39"/>
-      <c r="C63" s="40"/>
-      <c r="D63" s="41"/>
-      <c r="E63" s="41"/>
+      <c r="A63" s="26"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="25"/>
       <c r="F63" s="3" t="s">
         <v>32</v>
       </c>
@@ -9822,15 +9810,15 @@
       <c r="L63" t="s">
         <v>57</v>
       </c>
-      <c r="M63" s="45"/>
-      <c r="N63" s="46"/>
+      <c r="M63" s="22"/>
+      <c r="N63" s="23"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A64" s="38"/>
-      <c r="B64" s="39"/>
-      <c r="C64" s="40"/>
-      <c r="D64" s="41"/>
-      <c r="E64" s="41"/>
+      <c r="A64" s="26"/>
+      <c r="B64" s="27"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="25"/>
       <c r="F64" s="3" t="s">
         <v>33</v>
       </c>
@@ -9849,15 +9837,15 @@
       <c r="L64" t="s">
         <v>57</v>
       </c>
-      <c r="M64" s="45"/>
-      <c r="N64" s="46"/>
+      <c r="M64" s="22"/>
+      <c r="N64" s="23"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A65" s="38"/>
-      <c r="B65" s="39"/>
-      <c r="C65" s="40"/>
-      <c r="D65" s="41"/>
-      <c r="E65" s="41"/>
+      <c r="A65" s="26"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
       <c r="F65" s="3" t="s">
         <v>34</v>
       </c>
@@ -9876,15 +9864,15 @@
       <c r="L65" t="s">
         <v>57</v>
       </c>
-      <c r="M65" s="45"/>
-      <c r="N65" s="46"/>
+      <c r="M65" s="22"/>
+      <c r="N65" s="23"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A66" s="38"/>
-      <c r="B66" s="39"/>
-      <c r="C66" s="40"/>
-      <c r="D66" s="41"/>
-      <c r="E66" s="41"/>
+      <c r="A66" s="26"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="28"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
       <c r="F66" s="3" t="s">
         <v>35</v>
       </c>
@@ -9903,15 +9891,15 @@
       <c r="L66" t="s">
         <v>57</v>
       </c>
-      <c r="M66" s="45"/>
-      <c r="N66" s="46"/>
+      <c r="M66" s="22"/>
+      <c r="N66" s="23"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A67" s="38"/>
-      <c r="B67" s="39"/>
-      <c r="C67" s="40"/>
-      <c r="D67" s="41"/>
-      <c r="E67" s="41"/>
+      <c r="A67" s="26"/>
+      <c r="B67" s="27"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="25"/>
       <c r="F67" s="3" t="s">
         <v>36</v>
       </c>
@@ -9924,15 +9912,15 @@
       <c r="I67" t="s">
         <v>102</v>
       </c>
-      <c r="M67" s="45"/>
-      <c r="N67" s="46"/>
+      <c r="M67" s="22"/>
+      <c r="N67" s="23"/>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A68" s="38"/>
-      <c r="B68" s="39"/>
-      <c r="C68" s="40"/>
-      <c r="D68" s="41"/>
-      <c r="E68" s="41"/>
+      <c r="A68" s="26"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="25"/>
       <c r="F68" s="3" t="s">
         <v>37</v>
       </c>
@@ -9951,23 +9939,23 @@
       <c r="L68" t="s">
         <v>57</v>
       </c>
-      <c r="M68" s="45"/>
-      <c r="N68" s="46"/>
+      <c r="M68" s="22"/>
+      <c r="N68" s="23"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A69" s="38">
+      <c r="A69" s="26">
         <v>14</v>
       </c>
-      <c r="B69" s="39" t="s">
+      <c r="B69" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C69" s="40" t="s">
+      <c r="C69" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D69" s="41" t="s">
+      <c r="D69" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E69" s="41" t="s">
+      <c r="E69" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F69" s="3" t="s">
@@ -9982,16 +9970,16 @@
       <c r="I69" t="s">
         <v>77</v>
       </c>
-      <c r="M69" s="45" t="s">
+      <c r="M69" s="22" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A70" s="38"/>
-      <c r="B70" s="39"/>
-      <c r="C70" s="40"/>
-      <c r="D70" s="41"/>
-      <c r="E70" s="41"/>
+      <c r="A70" s="26"/>
+      <c r="B70" s="27"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="25"/>
       <c r="F70" s="3" t="s">
         <v>32</v>
       </c>
@@ -10008,19 +9996,19 @@
         <v>74</v>
       </c>
       <c r="L70" t="s">
-        <v>57</v>
-      </c>
-      <c r="M70" s="45"/>
+        <v>58</v>
+      </c>
+      <c r="M70" s="22"/>
       <c r="N70" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A71" s="38"/>
-      <c r="B71" s="39"/>
-      <c r="C71" s="40"/>
-      <c r="D71" s="41"/>
-      <c r="E71" s="41"/>
+      <c r="A71" s="26"/>
+      <c r="B71" s="27"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="25"/>
+      <c r="E71" s="25"/>
       <c r="F71" s="3" t="s">
         <v>33</v>
       </c>
@@ -10037,19 +10025,19 @@
         <v>74</v>
       </c>
       <c r="L71" t="s">
-        <v>57</v>
-      </c>
-      <c r="M71" s="45"/>
+        <v>58</v>
+      </c>
+      <c r="M71" s="22"/>
       <c r="N71" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A72" s="38"/>
-      <c r="B72" s="39"/>
-      <c r="C72" s="40"/>
-      <c r="D72" s="41"/>
-      <c r="E72" s="41"/>
+      <c r="A72" s="26"/>
+      <c r="B72" s="27"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="25"/>
+      <c r="E72" s="25"/>
       <c r="F72" s="3" t="s">
         <v>34</v>
       </c>
@@ -10066,19 +10054,19 @@
         <v>74</v>
       </c>
       <c r="L72" t="s">
-        <v>57</v>
-      </c>
-      <c r="M72" s="45"/>
+        <v>58</v>
+      </c>
+      <c r="M72" s="22"/>
       <c r="N72" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A73" s="38"/>
-      <c r="B73" s="39"/>
-      <c r="C73" s="40"/>
-      <c r="D73" s="41"/>
-      <c r="E73" s="41"/>
+      <c r="A73" s="26"/>
+      <c r="B73" s="27"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="25"/>
+      <c r="E73" s="25"/>
       <c r="F73" s="3" t="s">
         <v>35</v>
       </c>
@@ -10091,17 +10079,17 @@
       <c r="I73" t="s">
         <v>98</v>
       </c>
-      <c r="M73" s="45"/>
+      <c r="M73" s="22"/>
       <c r="N73" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A74" s="38"/>
-      <c r="B74" s="39"/>
-      <c r="C74" s="40"/>
-      <c r="D74" s="41"/>
-      <c r="E74" s="41"/>
+      <c r="A74" s="26"/>
+      <c r="B74" s="27"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="25"/>
+      <c r="E74" s="25"/>
       <c r="F74" s="3" t="s">
         <v>36</v>
       </c>
@@ -10118,19 +10106,19 @@
         <v>74</v>
       </c>
       <c r="L74" t="s">
-        <v>57</v>
-      </c>
-      <c r="M74" s="45"/>
+        <v>58</v>
+      </c>
+      <c r="M74" s="22"/>
       <c r="N74" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A75" s="38"/>
-      <c r="B75" s="39"/>
-      <c r="C75" s="40"/>
-      <c r="D75" s="41"/>
-      <c r="E75" s="41"/>
+      <c r="A75" s="26"/>
+      <c r="B75" s="27"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="25"/>
+      <c r="E75" s="25"/>
       <c r="F75" s="3" t="s">
         <v>37</v>
       </c>
@@ -10143,25 +10131,25 @@
       <c r="I75" t="s">
         <v>104</v>
       </c>
-      <c r="M75" s="45"/>
+      <c r="M75" s="22"/>
       <c r="N75" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A76" s="38">
+      <c r="A76" s="26">
         <v>16</v>
       </c>
-      <c r="B76" s="39" t="s">
+      <c r="B76" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C76" s="40" t="s">
+      <c r="C76" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D76" s="41" t="s">
+      <c r="D76" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E76" s="41" t="s">
+      <c r="E76" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F76" s="3" t="s">
@@ -10179,19 +10167,19 @@
       <c r="K76" t="s">
         <v>74</v>
       </c>
-      <c r="M76" s="45" t="s">
+      <c r="M76" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="N76" s="46">
+      <c r="N76" s="23">
         <v>45142</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A77" s="38"/>
-      <c r="B77" s="39"/>
-      <c r="C77" s="40"/>
-      <c r="D77" s="41"/>
-      <c r="E77" s="41"/>
+      <c r="A77" s="26"/>
+      <c r="B77" s="27"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="25"/>
+      <c r="E77" s="25"/>
       <c r="F77" s="3" t="s">
         <v>32</v>
       </c>
@@ -10207,15 +10195,15 @@
       <c r="K77" t="s">
         <v>74</v>
       </c>
-      <c r="M77" s="45"/>
-      <c r="N77" s="43"/>
+      <c r="M77" s="22"/>
+      <c r="N77" s="24"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A78" s="38"/>
-      <c r="B78" s="39"/>
-      <c r="C78" s="40"/>
-      <c r="D78" s="41"/>
-      <c r="E78" s="41"/>
+      <c r="A78" s="26"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="28"/>
+      <c r="D78" s="25"/>
+      <c r="E78" s="25"/>
       <c r="F78" s="3" t="s">
         <v>33</v>
       </c>
@@ -10232,17 +10220,17 @@
         <v>74</v>
       </c>
       <c r="L78" t="s">
-        <v>57</v>
-      </c>
-      <c r="M78" s="45"/>
-      <c r="N78" s="43"/>
+        <v>58</v>
+      </c>
+      <c r="M78" s="22"/>
+      <c r="N78" s="24"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A79" s="38"/>
-      <c r="B79" s="39"/>
-      <c r="C79" s="40"/>
-      <c r="D79" s="41"/>
-      <c r="E79" s="41"/>
+      <c r="A79" s="26"/>
+      <c r="B79" s="27"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="25"/>
+      <c r="E79" s="25"/>
       <c r="F79" s="3" t="s">
         <v>34</v>
       </c>
@@ -10259,17 +10247,17 @@
         <v>74</v>
       </c>
       <c r="L79" t="s">
-        <v>57</v>
-      </c>
-      <c r="M79" s="45"/>
-      <c r="N79" s="43"/>
+        <v>58</v>
+      </c>
+      <c r="M79" s="22"/>
+      <c r="N79" s="24"/>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A80" s="38"/>
-      <c r="B80" s="39"/>
-      <c r="C80" s="40"/>
-      <c r="D80" s="41"/>
-      <c r="E80" s="41"/>
+      <c r="A80" s="26"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="25"/>
       <c r="F80" s="3" t="s">
         <v>35</v>
       </c>
@@ -10285,15 +10273,15 @@
       <c r="K80" t="s">
         <v>74</v>
       </c>
-      <c r="M80" s="45"/>
-      <c r="N80" s="43"/>
+      <c r="M80" s="22"/>
+      <c r="N80" s="24"/>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A81" s="38"/>
-      <c r="B81" s="39"/>
-      <c r="C81" s="40"/>
-      <c r="D81" s="41"/>
-      <c r="E81" s="41"/>
+      <c r="A81" s="26"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="25"/>
+      <c r="E81" s="25"/>
       <c r="F81" s="3" t="s">
         <v>36</v>
       </c>
@@ -10310,17 +10298,17 @@
         <v>74</v>
       </c>
       <c r="L81" t="s">
-        <v>57</v>
-      </c>
-      <c r="M81" s="45"/>
-      <c r="N81" s="43"/>
+        <v>58</v>
+      </c>
+      <c r="M81" s="22"/>
+      <c r="N81" s="24"/>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A82" s="38"/>
-      <c r="B82" s="39"/>
-      <c r="C82" s="40"/>
-      <c r="D82" s="41"/>
-      <c r="E82" s="41"/>
+      <c r="A82" s="26"/>
+      <c r="B82" s="27"/>
+      <c r="C82" s="28"/>
+      <c r="D82" s="25"/>
+      <c r="E82" s="25"/>
       <c r="F82" s="3" t="s">
         <v>37</v>
       </c>
@@ -10336,23 +10324,23 @@
       <c r="K82" t="s">
         <v>74</v>
       </c>
-      <c r="M82" s="45"/>
-      <c r="N82" s="43"/>
+      <c r="M82" s="22"/>
+      <c r="N82" s="24"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A83" s="38">
+      <c r="A83" s="26">
         <v>17</v>
       </c>
-      <c r="B83" s="39" t="s">
+      <c r="B83" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C83" s="40" t="s">
+      <c r="C83" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="D83" s="41" t="s">
+      <c r="D83" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E83" s="41" t="s">
+      <c r="E83" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F83" s="3" t="s">
@@ -10370,19 +10358,19 @@
       <c r="K83" t="s">
         <v>74</v>
       </c>
-      <c r="M83" s="45" t="s">
+      <c r="M83" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="N83" s="46">
+      <c r="N83" s="23">
         <v>45142</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A84" s="38"/>
-      <c r="B84" s="39"/>
-      <c r="C84" s="40"/>
-      <c r="D84" s="41"/>
-      <c r="E84" s="41"/>
+      <c r="A84" s="26"/>
+      <c r="B84" s="27"/>
+      <c r="C84" s="28"/>
+      <c r="D84" s="25"/>
+      <c r="E84" s="25"/>
       <c r="F84" s="3" t="s">
         <v>32</v>
       </c>
@@ -10401,15 +10389,15 @@
       <c r="L84" t="s">
         <v>57</v>
       </c>
-      <c r="M84" s="43"/>
-      <c r="N84" s="43"/>
+      <c r="M84" s="24"/>
+      <c r="N84" s="24"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A85" s="38"/>
-      <c r="B85" s="39"/>
-      <c r="C85" s="40"/>
-      <c r="D85" s="41"/>
-      <c r="E85" s="41"/>
+      <c r="A85" s="26"/>
+      <c r="B85" s="27"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="25"/>
+      <c r="E85" s="25"/>
       <c r="F85" s="3" t="s">
         <v>33</v>
       </c>
@@ -10428,15 +10416,15 @@
       <c r="L85" t="s">
         <v>57</v>
       </c>
-      <c r="M85" s="43"/>
-      <c r="N85" s="43"/>
+      <c r="M85" s="24"/>
+      <c r="N85" s="24"/>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A86" s="38"/>
-      <c r="B86" s="39"/>
-      <c r="C86" s="40"/>
-      <c r="D86" s="41"/>
-      <c r="E86" s="41"/>
+      <c r="A86" s="26"/>
+      <c r="B86" s="27"/>
+      <c r="C86" s="28"/>
+      <c r="D86" s="25"/>
+      <c r="E86" s="25"/>
       <c r="F86" s="3" t="s">
         <v>34</v>
       </c>
@@ -10455,15 +10443,15 @@
       <c r="L86" t="s">
         <v>57</v>
       </c>
-      <c r="M86" s="43"/>
-      <c r="N86" s="43"/>
+      <c r="M86" s="24"/>
+      <c r="N86" s="24"/>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A87" s="38"/>
-      <c r="B87" s="39"/>
-      <c r="C87" s="40"/>
-      <c r="D87" s="41"/>
-      <c r="E87" s="41"/>
+      <c r="A87" s="26"/>
+      <c r="B87" s="27"/>
+      <c r="C87" s="28"/>
+      <c r="D87" s="25"/>
+      <c r="E87" s="25"/>
       <c r="F87" s="3" t="s">
         <v>35</v>
       </c>
@@ -10479,15 +10467,15 @@
       <c r="K87" t="s">
         <v>74</v>
       </c>
-      <c r="M87" s="43"/>
-      <c r="N87" s="43"/>
+      <c r="M87" s="24"/>
+      <c r="N87" s="24"/>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A88" s="38"/>
-      <c r="B88" s="39"/>
-      <c r="C88" s="40"/>
-      <c r="D88" s="41"/>
-      <c r="E88" s="41"/>
+      <c r="A88" s="26"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="25"/>
+      <c r="E88" s="25"/>
       <c r="F88" s="3" t="s">
         <v>36</v>
       </c>
@@ -10506,15 +10494,15 @@
       <c r="L88" t="s">
         <v>57</v>
       </c>
-      <c r="M88" s="43"/>
-      <c r="N88" s="43"/>
+      <c r="M88" s="24"/>
+      <c r="N88" s="24"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A89" s="38"/>
-      <c r="B89" s="39"/>
-      <c r="C89" s="40"/>
-      <c r="D89" s="41"/>
-      <c r="E89" s="41"/>
+      <c r="A89" s="26"/>
+      <c r="B89" s="27"/>
+      <c r="C89" s="28"/>
+      <c r="D89" s="25"/>
+      <c r="E89" s="25"/>
       <c r="F89" s="3" t="s">
         <v>37</v>
       </c>
@@ -10527,23 +10515,23 @@
       <c r="I89" t="s">
         <v>104</v>
       </c>
-      <c r="M89" s="43"/>
-      <c r="N89" s="43"/>
+      <c r="M89" s="24"/>
+      <c r="N89" s="24"/>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A90" s="38">
+      <c r="A90" s="26">
         <v>18</v>
       </c>
-      <c r="B90" s="39" t="s">
+      <c r="B90" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C90" s="40" t="s">
+      <c r="C90" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D90" s="41" t="s">
+      <c r="D90" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E90" s="41" t="s">
+      <c r="E90" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F90" s="3" t="s">
@@ -10564,19 +10552,19 @@
       <c r="L90" t="s">
         <v>57</v>
       </c>
-      <c r="M90" s="45" t="s">
-        <v>125</v>
-      </c>
-      <c r="N90" s="46">
+      <c r="M90" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="N90" s="23">
         <v>45145</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A91" s="38"/>
-      <c r="B91" s="39"/>
-      <c r="C91" s="40"/>
-      <c r="D91" s="41"/>
-      <c r="E91" s="41"/>
+      <c r="A91" s="26"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="28"/>
+      <c r="D91" s="25"/>
+      <c r="E91" s="25"/>
       <c r="F91" s="3" t="s">
         <v>32</v>
       </c>
@@ -10595,15 +10583,15 @@
       <c r="L91" t="s">
         <v>57</v>
       </c>
-      <c r="M91" s="45"/>
-      <c r="N91" s="46"/>
+      <c r="M91" s="22"/>
+      <c r="N91" s="23"/>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A92" s="38"/>
-      <c r="B92" s="39"/>
-      <c r="C92" s="40"/>
-      <c r="D92" s="41"/>
-      <c r="E92" s="41"/>
+      <c r="A92" s="26"/>
+      <c r="B92" s="27"/>
+      <c r="C92" s="28"/>
+      <c r="D92" s="25"/>
+      <c r="E92" s="25"/>
       <c r="F92" s="3" t="s">
         <v>33</v>
       </c>
@@ -10622,15 +10610,15 @@
       <c r="L92" t="s">
         <v>57</v>
       </c>
-      <c r="M92" s="45"/>
-      <c r="N92" s="46"/>
+      <c r="M92" s="22"/>
+      <c r="N92" s="23"/>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A93" s="38"/>
-      <c r="B93" s="39"/>
-      <c r="C93" s="40"/>
-      <c r="D93" s="41"/>
-      <c r="E93" s="41"/>
+      <c r="A93" s="26"/>
+      <c r="B93" s="27"/>
+      <c r="C93" s="28"/>
+      <c r="D93" s="25"/>
+      <c r="E93" s="25"/>
       <c r="F93" s="3" t="s">
         <v>34</v>
       </c>
@@ -10649,15 +10637,15 @@
       <c r="L93" t="s">
         <v>57</v>
       </c>
-      <c r="M93" s="45"/>
-      <c r="N93" s="46"/>
+      <c r="M93" s="22"/>
+      <c r="N93" s="23"/>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A94" s="38"/>
-      <c r="B94" s="39"/>
-      <c r="C94" s="40"/>
-      <c r="D94" s="41"/>
-      <c r="E94" s="41"/>
+      <c r="A94" s="26"/>
+      <c r="B94" s="27"/>
+      <c r="C94" s="28"/>
+      <c r="D94" s="25"/>
+      <c r="E94" s="25"/>
       <c r="F94" s="3" t="s">
         <v>35</v>
       </c>
@@ -10673,15 +10661,15 @@
       <c r="K94" t="s">
         <v>74</v>
       </c>
-      <c r="M94" s="45"/>
-      <c r="N94" s="46"/>
+      <c r="M94" s="22"/>
+      <c r="N94" s="23"/>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A95" s="38"/>
-      <c r="B95" s="39"/>
-      <c r="C95" s="40"/>
-      <c r="D95" s="41"/>
-      <c r="E95" s="41"/>
+      <c r="A95" s="26"/>
+      <c r="B95" s="27"/>
+      <c r="C95" s="28"/>
+      <c r="D95" s="25"/>
+      <c r="E95" s="25"/>
       <c r="F95" s="3" t="s">
         <v>36</v>
       </c>
@@ -10700,15 +10688,15 @@
       <c r="L95" t="s">
         <v>57</v>
       </c>
-      <c r="M95" s="45"/>
-      <c r="N95" s="46"/>
+      <c r="M95" s="22"/>
+      <c r="N95" s="23"/>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A96" s="38"/>
-      <c r="B96" s="39"/>
-      <c r="C96" s="40"/>
-      <c r="D96" s="41"/>
-      <c r="E96" s="41"/>
+      <c r="A96" s="26"/>
+      <c r="B96" s="27"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="25"/>
+      <c r="E96" s="25"/>
       <c r="F96" s="3" t="s">
         <v>37</v>
       </c>
@@ -10721,23 +10709,23 @@
       <c r="I96" t="s">
         <v>104</v>
       </c>
-      <c r="M96" s="45"/>
-      <c r="N96" s="46"/>
+      <c r="M96" s="22"/>
+      <c r="N96" s="23"/>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A97" s="38">
+      <c r="A97" s="26">
         <v>19</v>
       </c>
-      <c r="B97" s="39" t="s">
+      <c r="B97" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C97" s="40" t="s">
+      <c r="C97" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D97" s="41" t="s">
+      <c r="D97" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E97" s="41" t="s">
+      <c r="E97" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F97" s="3" t="s">
@@ -10756,26 +10744,26 @@
         <v>74</v>
       </c>
       <c r="L97" t="s">
-        <v>57</v>
-      </c>
-      <c r="M97" s="45" t="s">
-        <v>127</v>
-      </c>
-      <c r="N97" s="46">
+        <v>58</v>
+      </c>
+      <c r="M97" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="N97" s="23">
         <v>45145</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A98" s="38"/>
-      <c r="B98" s="39"/>
-      <c r="C98" s="40"/>
-      <c r="D98" s="41"/>
-      <c r="E98" s="41"/>
+      <c r="A98" s="26"/>
+      <c r="B98" s="27"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="25"/>
+      <c r="E98" s="25"/>
       <c r="F98" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G98" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H98" t="s">
         <v>118</v>
@@ -10787,22 +10775,22 @@
         <v>74</v>
       </c>
       <c r="L98" t="s">
-        <v>57</v>
-      </c>
-      <c r="M98" s="45"/>
-      <c r="N98" s="46"/>
+        <v>58</v>
+      </c>
+      <c r="M98" s="22"/>
+      <c r="N98" s="23"/>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A99" s="38"/>
-      <c r="B99" s="39"/>
-      <c r="C99" s="40"/>
-      <c r="D99" s="41"/>
-      <c r="E99" s="41"/>
+      <c r="A99" s="26"/>
+      <c r="B99" s="27"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="25"/>
+      <c r="E99" s="25"/>
       <c r="F99" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G99" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H99" t="s">
         <v>117</v>
@@ -10814,22 +10802,22 @@
         <v>74</v>
       </c>
       <c r="L99" t="s">
-        <v>57</v>
-      </c>
-      <c r="M99" s="45"/>
-      <c r="N99" s="46"/>
+        <v>58</v>
+      </c>
+      <c r="M99" s="22"/>
+      <c r="N99" s="23"/>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A100" s="38"/>
-      <c r="B100" s="39"/>
-      <c r="C100" s="40"/>
-      <c r="D100" s="41"/>
-      <c r="E100" s="41"/>
+      <c r="A100" s="26"/>
+      <c r="B100" s="27"/>
+      <c r="C100" s="28"/>
+      <c r="D100" s="25"/>
+      <c r="E100" s="25"/>
       <c r="F100" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G100" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H100" t="s">
         <v>117</v>
@@ -10841,17 +10829,17 @@
         <v>74</v>
       </c>
       <c r="L100" t="s">
-        <v>57</v>
-      </c>
-      <c r="M100" s="45"/>
-      <c r="N100" s="46"/>
+        <v>58</v>
+      </c>
+      <c r="M100" s="22"/>
+      <c r="N100" s="23"/>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A101" s="38"/>
-      <c r="B101" s="39"/>
-      <c r="C101" s="40"/>
-      <c r="D101" s="41"/>
-      <c r="E101" s="41"/>
+      <c r="A101" s="26"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="28"/>
+      <c r="D101" s="25"/>
+      <c r="E101" s="25"/>
       <c r="F101" s="3" t="s">
         <v>35</v>
       </c>
@@ -10867,20 +10855,20 @@
       <c r="K101" t="s">
         <v>74</v>
       </c>
-      <c r="M101" s="45"/>
-      <c r="N101" s="46"/>
+      <c r="M101" s="22"/>
+      <c r="N101" s="23"/>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A102" s="38"/>
-      <c r="B102" s="39"/>
-      <c r="C102" s="40"/>
-      <c r="D102" s="41"/>
-      <c r="E102" s="41"/>
+      <c r="A102" s="26"/>
+      <c r="B102" s="27"/>
+      <c r="C102" s="28"/>
+      <c r="D102" s="25"/>
+      <c r="E102" s="25"/>
       <c r="F102" s="3" t="s">
         <v>36</v>
       </c>
       <c r="G102" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H102" t="s">
         <v>106</v>
@@ -10892,17 +10880,17 @@
         <v>74</v>
       </c>
       <c r="L102" t="s">
-        <v>57</v>
-      </c>
-      <c r="M102" s="45"/>
-      <c r="N102" s="46"/>
+        <v>58</v>
+      </c>
+      <c r="M102" s="22"/>
+      <c r="N102" s="23"/>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A103" s="38"/>
-      <c r="B103" s="39"/>
-      <c r="C103" s="40"/>
-      <c r="D103" s="41"/>
-      <c r="E103" s="41"/>
+      <c r="A103" s="26"/>
+      <c r="B103" s="27"/>
+      <c r="C103" s="28"/>
+      <c r="D103" s="25"/>
+      <c r="E103" s="25"/>
       <c r="F103" s="3" t="s">
         <v>37</v>
       </c>
@@ -10915,23 +10903,23 @@
       <c r="I103" t="s">
         <v>104</v>
       </c>
-      <c r="M103" s="45"/>
-      <c r="N103" s="46"/>
+      <c r="M103" s="22"/>
+      <c r="N103" s="23"/>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A104" s="38">
+      <c r="A104" s="26">
         <v>29</v>
       </c>
-      <c r="B104" s="39" t="s">
+      <c r="B104" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C104" s="40" t="s">
+      <c r="C104" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D104" s="41" t="s">
+      <c r="D104" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E104" s="41" t="s">
+      <c r="E104" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F104" s="3" t="s">
@@ -10946,7 +10934,7 @@
       <c r="K104" t="s">
         <v>74</v>
       </c>
-      <c r="M104" s="45" t="s">
+      <c r="M104" s="22" t="s">
         <v>115</v>
       </c>
       <c r="N104" s="1">
@@ -10954,16 +10942,16 @@
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A105" s="38"/>
-      <c r="B105" s="39"/>
-      <c r="C105" s="40"/>
-      <c r="D105" s="41"/>
-      <c r="E105" s="41"/>
+      <c r="A105" s="26"/>
+      <c r="B105" s="27"/>
+      <c r="C105" s="28"/>
+      <c r="D105" s="25"/>
+      <c r="E105" s="25"/>
       <c r="F105" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G105" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H105" t="s">
         <v>114</v>
@@ -10975,24 +10963,24 @@
         <v>74</v>
       </c>
       <c r="L105" t="s">
-        <v>57</v>
-      </c>
-      <c r="M105" s="45"/>
+        <v>58</v>
+      </c>
+      <c r="M105" s="22"/>
       <c r="N105" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A106" s="38"/>
-      <c r="B106" s="39"/>
-      <c r="C106" s="40"/>
-      <c r="D106" s="41"/>
-      <c r="E106" s="41"/>
+      <c r="A106" s="26"/>
+      <c r="B106" s="27"/>
+      <c r="C106" s="28"/>
+      <c r="D106" s="25"/>
+      <c r="E106" s="25"/>
       <c r="F106" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G106" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H106" t="s">
         <v>112</v>
@@ -11004,24 +10992,24 @@
         <v>74</v>
       </c>
       <c r="L106" t="s">
-        <v>57</v>
-      </c>
-      <c r="M106" s="45"/>
+        <v>58</v>
+      </c>
+      <c r="M106" s="22"/>
       <c r="N106" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A107" s="38"/>
-      <c r="B107" s="39"/>
-      <c r="C107" s="40"/>
-      <c r="D107" s="41"/>
-      <c r="E107" s="41"/>
+      <c r="A107" s="26"/>
+      <c r="B107" s="27"/>
+      <c r="C107" s="28"/>
+      <c r="D107" s="25"/>
+      <c r="E107" s="25"/>
       <c r="F107" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G107" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H107" t="s">
         <v>112</v>
@@ -11033,19 +11021,19 @@
         <v>74</v>
       </c>
       <c r="L107" t="s">
-        <v>57</v>
-      </c>
-      <c r="M107" s="45"/>
+        <v>58</v>
+      </c>
+      <c r="M107" s="22"/>
       <c r="N107" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A108" s="38"/>
-      <c r="B108" s="39"/>
-      <c r="C108" s="40"/>
-      <c r="D108" s="41"/>
-      <c r="E108" s="41"/>
+      <c r="A108" s="26"/>
+      <c r="B108" s="27"/>
+      <c r="C108" s="28"/>
+      <c r="D108" s="25"/>
+      <c r="E108" s="25"/>
       <c r="F108" s="3" t="s">
         <v>35</v>
       </c>
@@ -11061,22 +11049,22 @@
       <c r="L108" t="s">
         <v>57</v>
       </c>
-      <c r="M108" s="45"/>
+      <c r="M108" s="22"/>
       <c r="N108" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A109" s="38"/>
-      <c r="B109" s="39"/>
-      <c r="C109" s="40"/>
-      <c r="D109" s="41"/>
-      <c r="E109" s="41"/>
+      <c r="A109" s="26"/>
+      <c r="B109" s="27"/>
+      <c r="C109" s="28"/>
+      <c r="D109" s="25"/>
+      <c r="E109" s="25"/>
       <c r="F109" s="3" t="s">
         <v>36</v>
       </c>
       <c r="G109" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H109" t="s">
         <v>106</v>
@@ -11088,19 +11076,19 @@
         <v>74</v>
       </c>
       <c r="L109" t="s">
-        <v>57</v>
-      </c>
-      <c r="M109" s="45"/>
+        <v>58</v>
+      </c>
+      <c r="M109" s="22"/>
       <c r="N109" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A110" s="38"/>
-      <c r="B110" s="39"/>
-      <c r="C110" s="40"/>
-      <c r="D110" s="41"/>
-      <c r="E110" s="41"/>
+      <c r="A110" s="26"/>
+      <c r="B110" s="27"/>
+      <c r="C110" s="28"/>
+      <c r="D110" s="25"/>
+      <c r="E110" s="25"/>
       <c r="F110" s="3" t="s">
         <v>37</v>
       </c>
@@ -11113,25 +11101,25 @@
       <c r="I110" t="s">
         <v>104</v>
       </c>
-      <c r="M110" s="45"/>
+      <c r="M110" s="22"/>
       <c r="N110" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A111" s="38">
+      <c r="A111" s="26">
         <v>29</v>
       </c>
-      <c r="B111" s="39" t="s">
+      <c r="B111" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C111" s="40" t="s">
+      <c r="C111" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="D111" s="41" t="s">
+      <c r="D111" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E111" s="41" t="s">
+      <c r="E111" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F111" s="3" t="s">
@@ -11149,19 +11137,19 @@
       <c r="L111" t="s">
         <v>57</v>
       </c>
-      <c r="M111" s="44" t="s">
-        <v>123</v>
+      <c r="M111" s="29" t="s">
+        <v>132</v>
       </c>
       <c r="N111" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A112" s="38"/>
-      <c r="B112" s="39"/>
-      <c r="C112" s="40"/>
-      <c r="D112" s="41"/>
-      <c r="E112" s="41"/>
+      <c r="A112" s="26"/>
+      <c r="B112" s="27"/>
+      <c r="C112" s="28"/>
+      <c r="D112" s="25"/>
+      <c r="E112" s="25"/>
       <c r="F112" s="3" t="s">
         <v>32</v>
       </c>
@@ -11180,17 +11168,17 @@
       <c r="L112" t="s">
         <v>57</v>
       </c>
-      <c r="M112" s="42"/>
+      <c r="M112" s="30"/>
       <c r="N112" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A113" s="38"/>
-      <c r="B113" s="39"/>
-      <c r="C113" s="40"/>
-      <c r="D113" s="41"/>
-      <c r="E113" s="41"/>
+      <c r="A113" s="26"/>
+      <c r="B113" s="27"/>
+      <c r="C113" s="28"/>
+      <c r="D113" s="25"/>
+      <c r="E113" s="25"/>
       <c r="F113" s="3" t="s">
         <v>33</v>
       </c>
@@ -11209,17 +11197,17 @@
       <c r="L113" t="s">
         <v>57</v>
       </c>
-      <c r="M113" s="42"/>
+      <c r="M113" s="30"/>
       <c r="N113" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A114" s="38"/>
-      <c r="B114" s="39"/>
-      <c r="C114" s="40"/>
-      <c r="D114" s="41"/>
-      <c r="E114" s="41"/>
+      <c r="A114" s="26"/>
+      <c r="B114" s="27"/>
+      <c r="C114" s="28"/>
+      <c r="D114" s="25"/>
+      <c r="E114" s="25"/>
       <c r="F114" s="3" t="s">
         <v>34</v>
       </c>
@@ -11238,17 +11226,17 @@
       <c r="L114" t="s">
         <v>57</v>
       </c>
-      <c r="M114" s="42"/>
+      <c r="M114" s="30"/>
       <c r="N114" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A115" s="38"/>
-      <c r="B115" s="39"/>
-      <c r="C115" s="40"/>
-      <c r="D115" s="41"/>
-      <c r="E115" s="41"/>
+      <c r="A115" s="26"/>
+      <c r="B115" s="27"/>
+      <c r="C115" s="28"/>
+      <c r="D115" s="25"/>
+      <c r="E115" s="25"/>
       <c r="F115" s="3" t="s">
         <v>35</v>
       </c>
@@ -11264,17 +11252,17 @@
       <c r="L115" t="s">
         <v>57</v>
       </c>
-      <c r="M115" s="42"/>
+      <c r="M115" s="30"/>
       <c r="N115" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A116" s="38"/>
-      <c r="B116" s="39"/>
-      <c r="C116" s="40"/>
-      <c r="D116" s="41"/>
-      <c r="E116" s="41"/>
+      <c r="A116" s="26"/>
+      <c r="B116" s="27"/>
+      <c r="C116" s="28"/>
+      <c r="D116" s="25"/>
+      <c r="E116" s="25"/>
       <c r="F116" s="3" t="s">
         <v>36</v>
       </c>
@@ -11293,17 +11281,17 @@
       <c r="L116" t="s">
         <v>57</v>
       </c>
-      <c r="M116" s="42"/>
+      <c r="M116" s="30"/>
       <c r="N116" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A117" s="38"/>
-      <c r="B117" s="39"/>
-      <c r="C117" s="40"/>
-      <c r="D117" s="41"/>
-      <c r="E117" s="41"/>
+      <c r="A117" s="26"/>
+      <c r="B117" s="27"/>
+      <c r="C117" s="28"/>
+      <c r="D117" s="25"/>
+      <c r="E117" s="25"/>
       <c r="F117" s="3" t="s">
         <v>37</v>
       </c>
@@ -11316,24 +11304,88 @@
       <c r="I117" t="s">
         <v>104</v>
       </c>
-      <c r="M117" s="42"/>
+      <c r="M117" s="30"/>
       <c r="N117" s="1">
         <v>45142</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="G1:G117"/>
   <mergeCells count="109">
-    <mergeCell ref="M90:M96"/>
-    <mergeCell ref="N90:N96"/>
-    <mergeCell ref="M97:M103"/>
-    <mergeCell ref="N97:N103"/>
-    <mergeCell ref="M104:M110"/>
-    <mergeCell ref="N55:N61"/>
-    <mergeCell ref="M62:M68"/>
-    <mergeCell ref="N62:N68"/>
-    <mergeCell ref="M69:M75"/>
-    <mergeCell ref="M83:M89"/>
-    <mergeCell ref="N83:N89"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="C13:C19"/>
+    <mergeCell ref="D13:D19"/>
+    <mergeCell ref="E13:E19"/>
+    <mergeCell ref="A1:N2"/>
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="G3:N4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:B26"/>
+    <mergeCell ref="C20:C26"/>
+    <mergeCell ref="D20:D26"/>
+    <mergeCell ref="E20:E26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="B27:B33"/>
+    <mergeCell ref="C27:C33"/>
+    <mergeCell ref="D27:D33"/>
+    <mergeCell ref="E27:E33"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="C34:C40"/>
+    <mergeCell ref="D34:D40"/>
+    <mergeCell ref="E34:E40"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="B48:B54"/>
+    <mergeCell ref="C48:C54"/>
+    <mergeCell ref="D48:D54"/>
+    <mergeCell ref="E48:E54"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="C41:C47"/>
+    <mergeCell ref="D41:D47"/>
+    <mergeCell ref="E41:E47"/>
+    <mergeCell ref="C69:C75"/>
+    <mergeCell ref="D69:D75"/>
+    <mergeCell ref="E69:E75"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:B82"/>
+    <mergeCell ref="C76:C82"/>
+    <mergeCell ref="D76:D82"/>
+    <mergeCell ref="E76:E82"/>
+    <mergeCell ref="A83:A89"/>
+    <mergeCell ref="B83:B89"/>
+    <mergeCell ref="C83:C89"/>
+    <mergeCell ref="D83:D89"/>
+    <mergeCell ref="E83:E89"/>
+    <mergeCell ref="D104:D110"/>
+    <mergeCell ref="E104:E110"/>
+    <mergeCell ref="A97:A103"/>
+    <mergeCell ref="B97:B103"/>
+    <mergeCell ref="C97:C103"/>
+    <mergeCell ref="D97:D103"/>
+    <mergeCell ref="E97:E103"/>
+    <mergeCell ref="B55:B61"/>
+    <mergeCell ref="C55:C61"/>
+    <mergeCell ref="D55:D61"/>
+    <mergeCell ref="E55:E61"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="B62:B68"/>
+    <mergeCell ref="C62:C68"/>
+    <mergeCell ref="D62:D68"/>
+    <mergeCell ref="E62:E68"/>
+    <mergeCell ref="A90:A96"/>
+    <mergeCell ref="B90:B96"/>
+    <mergeCell ref="C90:C96"/>
+    <mergeCell ref="D90:D96"/>
+    <mergeCell ref="E90:E96"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:B75"/>
     <mergeCell ref="D111:D117"/>
     <mergeCell ref="E111:E117"/>
     <mergeCell ref="A111:A117"/>
@@ -11358,80 +11410,17 @@
     <mergeCell ref="A104:A110"/>
     <mergeCell ref="B104:B110"/>
     <mergeCell ref="C104:C110"/>
-    <mergeCell ref="D104:D110"/>
-    <mergeCell ref="E104:E110"/>
-    <mergeCell ref="A97:A103"/>
-    <mergeCell ref="B97:B103"/>
-    <mergeCell ref="C97:C103"/>
-    <mergeCell ref="D97:D103"/>
-    <mergeCell ref="E97:E103"/>
-    <mergeCell ref="B55:B61"/>
-    <mergeCell ref="C55:C61"/>
-    <mergeCell ref="D55:D61"/>
-    <mergeCell ref="E55:E61"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="B62:B68"/>
-    <mergeCell ref="C62:C68"/>
-    <mergeCell ref="D62:D68"/>
-    <mergeCell ref="E62:E68"/>
-    <mergeCell ref="A90:A96"/>
-    <mergeCell ref="B90:B96"/>
-    <mergeCell ref="C90:C96"/>
-    <mergeCell ref="D90:D96"/>
-    <mergeCell ref="E90:E96"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:B75"/>
-    <mergeCell ref="C69:C75"/>
-    <mergeCell ref="D69:D75"/>
-    <mergeCell ref="E69:E75"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:B82"/>
-    <mergeCell ref="C76:C82"/>
-    <mergeCell ref="D76:D82"/>
-    <mergeCell ref="E76:E82"/>
-    <mergeCell ref="A83:A89"/>
-    <mergeCell ref="B83:B89"/>
-    <mergeCell ref="C83:C89"/>
-    <mergeCell ref="D83:D89"/>
-    <mergeCell ref="E83:E89"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="B34:B40"/>
-    <mergeCell ref="C34:C40"/>
-    <mergeCell ref="D34:D40"/>
-    <mergeCell ref="E34:E40"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="B48:B54"/>
-    <mergeCell ref="C48:C54"/>
-    <mergeCell ref="D48:D54"/>
-    <mergeCell ref="E48:E54"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="B41:B47"/>
-    <mergeCell ref="C41:C47"/>
-    <mergeCell ref="D41:D47"/>
-    <mergeCell ref="E41:E47"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:B26"/>
-    <mergeCell ref="C20:C26"/>
-    <mergeCell ref="D20:D26"/>
-    <mergeCell ref="E20:E26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:B33"/>
-    <mergeCell ref="C27:C33"/>
-    <mergeCell ref="D27:D33"/>
-    <mergeCell ref="E27:E33"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B13:B19"/>
-    <mergeCell ref="C13:C19"/>
-    <mergeCell ref="D13:D19"/>
-    <mergeCell ref="E13:E19"/>
-    <mergeCell ref="A1:N2"/>
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="E3:F4"/>
-    <mergeCell ref="G3:N4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="M90:M96"/>
+    <mergeCell ref="N90:N96"/>
+    <mergeCell ref="M97:M103"/>
+    <mergeCell ref="N97:N103"/>
+    <mergeCell ref="M104:M110"/>
+    <mergeCell ref="N55:N61"/>
+    <mergeCell ref="M62:M68"/>
+    <mergeCell ref="N62:N68"/>
+    <mergeCell ref="M69:M75"/>
+    <mergeCell ref="M83:M89"/>
+    <mergeCell ref="N83:N89"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M11" r:id="rId1"/>
@@ -11443,7 +11432,7 @@
     <hyperlink ref="M104" r:id="rId7"/>
     <hyperlink ref="M41" r:id="rId8"/>
     <hyperlink ref="M69" r:id="rId9"/>
-    <hyperlink ref="M111" r:id="rId10"/>
+    <hyperlink ref="M111" r:id="rId10" display="https://pabmi.atlassian.net/browse/PABMI-813"/>
     <hyperlink ref="M55" r:id="rId11"/>
     <hyperlink ref="M90" r:id="rId12"/>
     <hyperlink ref="M27" r:id="rId13"/>

</xml_diff>

<commit_message>
Guía Configuración Catálogos PABMI
</commit_message>
<xml_diff>
--- a/PABMI/ENTREGABLES/Matriz de Pruebas Configuraciones Catálogos BIENES MUEBLES.xlsx
+++ b/PABMI/ENTREGABLES/Matriz de Pruebas Configuraciones Catálogos BIENES MUEBLES.xlsx
@@ -875,18 +875,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -896,14 +884,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -954,6 +936,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8049,10 +8049,10 @@
   <dimension ref="A1:N117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="7" ySplit="9" topLeftCell="H48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="9" topLeftCell="H60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G52" sqref="G52"/>
+      <selection pane="bottomRight" activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8073,94 +8073,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="39" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
@@ -8428,13 +8428,13 @@
       <c r="N12" s="21"/>
     </row>
     <row r="13" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="26">
+      <c r="A13" s="22">
         <v>7</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="24" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="25" t="s">
@@ -8456,17 +8456,17 @@
         <v>92</v>
       </c>
       <c r="J13" s="2"/>
-      <c r="M13" s="22" t="s">
+      <c r="M13" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="N13" s="23">
+      <c r="N13" s="46">
         <v>45142</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
       <c r="F14" s="3" t="s">
@@ -8480,13 +8480,13 @@
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="2"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="23"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="46"/>
     </row>
     <row r="15" spans="1:14" ht="33" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
       <c r="F15" s="3" t="s">
@@ -8508,13 +8508,13 @@
       <c r="L15" t="s">
         <v>58</v>
       </c>
-      <c r="M15" s="24"/>
-      <c r="N15" s="23"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="46"/>
     </row>
     <row r="16" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="25"/>
       <c r="E16" s="25"/>
       <c r="F16" s="3" t="s">
@@ -8536,13 +8536,13 @@
       <c r="L16" t="s">
         <v>58</v>
       </c>
-      <c r="M16" s="24"/>
-      <c r="N16" s="23"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="46"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="25"/>
       <c r="E17" s="25"/>
       <c r="F17" s="3" t="s">
@@ -8558,13 +8558,13 @@
         <v>98</v>
       </c>
       <c r="J17" s="2"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="23"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="46"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="26"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="25"/>
       <c r="E18" s="25"/>
       <c r="F18" s="3" t="s">
@@ -8586,13 +8586,13 @@
       <c r="L18" t="s">
         <v>58</v>
       </c>
-      <c r="M18" s="24"/>
-      <c r="N18" s="23"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="46"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
       <c r="F19" s="3" t="s">
@@ -8608,17 +8608,17 @@
         <v>104</v>
       </c>
       <c r="J19" s="2"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="23"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="46"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="26">
+      <c r="A20" s="22">
         <v>8</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="24" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="25" t="s">
@@ -8645,17 +8645,17 @@
       <c r="L20" t="s">
         <v>58</v>
       </c>
-      <c r="M20" s="29" t="s">
+      <c r="M20" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="N20" s="31">
+      <c r="N20" s="48">
         <v>45145</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="26"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="25"/>
       <c r="E21" s="25"/>
       <c r="F21" s="3" t="s">
@@ -8676,13 +8676,13 @@
       <c r="L21" t="s">
         <v>58</v>
       </c>
-      <c r="M21" s="30"/>
-      <c r="N21" s="31"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="48"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="26"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="25"/>
       <c r="E22" s="25"/>
       <c r="F22" s="3" t="s">
@@ -8703,13 +8703,13 @@
       <c r="L22" t="s">
         <v>58</v>
       </c>
-      <c r="M22" s="30"/>
-      <c r="N22" s="31"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="48"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="25"/>
       <c r="E23" s="25"/>
       <c r="F23" s="3" t="s">
@@ -8730,13 +8730,13 @@
       <c r="L23" t="s">
         <v>58</v>
       </c>
-      <c r="M23" s="30"/>
-      <c r="N23" s="31"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="48"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="26"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="25"/>
       <c r="E24" s="25"/>
       <c r="F24" s="3" t="s">
@@ -8751,13 +8751,13 @@
       <c r="I24" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="M24" s="30"/>
-      <c r="N24" s="31"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="48"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="28"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="25"/>
       <c r="E25" s="25"/>
       <c r="F25" s="3" t="s">
@@ -8778,13 +8778,13 @@
       <c r="L25" t="s">
         <v>58</v>
       </c>
-      <c r="M25" s="30"/>
-      <c r="N25" s="31"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="48"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="26"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="25"/>
       <c r="E26" s="25"/>
       <c r="F26" s="3" t="s">
@@ -8799,17 +8799,17 @@
       <c r="I26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="M26" s="30"/>
-      <c r="N26" s="31"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="48"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="26">
+      <c r="A27" s="22">
         <v>9</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D27" s="25" t="s">
@@ -8836,17 +8836,17 @@
       <c r="L27" t="s">
         <v>57</v>
       </c>
-      <c r="M27" s="22" t="s">
+      <c r="M27" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="N27" s="31">
+      <c r="N27" s="48">
         <v>45145</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="26"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="28"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="25"/>
       <c r="E28" s="25"/>
       <c r="F28" s="3" t="s">
@@ -8867,13 +8867,13 @@
       <c r="L28" t="s">
         <v>57</v>
       </c>
-      <c r="M28" s="22"/>
-      <c r="N28" s="31"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="48"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="25"/>
       <c r="E29" s="25"/>
       <c r="F29" s="3" t="s">
@@ -8894,13 +8894,13 @@
       <c r="L29" t="s">
         <v>57</v>
       </c>
-      <c r="M29" s="22"/>
-      <c r="N29" s="31"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="48"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="26"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="28"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="25"/>
       <c r="E30" s="25"/>
       <c r="F30" s="3" t="s">
@@ -8921,13 +8921,13 @@
       <c r="L30" t="s">
         <v>57</v>
       </c>
-      <c r="M30" s="22"/>
-      <c r="N30" s="31"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="48"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="28"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="24"/>
       <c r="D31" s="25"/>
       <c r="E31" s="25"/>
       <c r="F31" s="3" t="s">
@@ -8942,13 +8942,13 @@
       <c r="I31" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="M31" s="22"/>
-      <c r="N31" s="31"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="48"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" s="26"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="28"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="24"/>
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
       <c r="F32" s="3" t="s">
@@ -8969,13 +8969,13 @@
       <c r="L32" t="s">
         <v>57</v>
       </c>
-      <c r="M32" s="22"/>
-      <c r="N32" s="31"/>
+      <c r="M32" s="45"/>
+      <c r="N32" s="48"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="26"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="28"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="24"/>
       <c r="D33" s="25"/>
       <c r="E33" s="25"/>
       <c r="F33" s="3" t="s">
@@ -8990,17 +8990,17 @@
       <c r="I33" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="M33" s="22"/>
-      <c r="N33" s="31"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="48"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="26">
+      <c r="A34" s="22">
         <v>10</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="24" t="s">
         <v>41</v>
       </c>
       <c r="D34" s="25" t="s">
@@ -9027,17 +9027,17 @@
       <c r="L34" t="s">
         <v>57</v>
       </c>
-      <c r="M34" s="29" t="s">
+      <c r="M34" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="N34" s="31">
+      <c r="N34" s="48">
         <v>45145</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="26"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="28"/>
+      <c r="A35" s="22"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="25"/>
       <c r="E35" s="25"/>
       <c r="F35" s="3" t="s">
@@ -9058,13 +9058,13 @@
       <c r="L35" t="s">
         <v>57</v>
       </c>
-      <c r="M35" s="30"/>
-      <c r="N35" s="31"/>
+      <c r="M35" s="44"/>
+      <c r="N35" s="48"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="26"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="28"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="25"/>
       <c r="E36" s="25"/>
       <c r="F36" s="3" t="s">
@@ -9085,13 +9085,13 @@
       <c r="L36" t="s">
         <v>57</v>
       </c>
-      <c r="M36" s="30"/>
-      <c r="N36" s="31"/>
+      <c r="M36" s="44"/>
+      <c r="N36" s="48"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="26"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="28"/>
+      <c r="A37" s="22"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="24"/>
       <c r="D37" s="25"/>
       <c r="E37" s="25"/>
       <c r="F37" s="3" t="s">
@@ -9112,13 +9112,13 @@
       <c r="L37" t="s">
         <v>57</v>
       </c>
-      <c r="M37" s="30"/>
-      <c r="N37" s="31"/>
+      <c r="M37" s="44"/>
+      <c r="N37" s="48"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="26"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="28"/>
+      <c r="A38" s="22"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="25"/>
       <c r="E38" s="25"/>
       <c r="F38" s="3" t="s">
@@ -9133,13 +9133,13 @@
       <c r="I38" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="M38" s="30"/>
-      <c r="N38" s="31"/>
+      <c r="M38" s="44"/>
+      <c r="N38" s="48"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="26"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="28"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="25"/>
       <c r="E39" s="25"/>
       <c r="F39" s="3" t="s">
@@ -9160,13 +9160,13 @@
       <c r="L39" t="s">
         <v>57</v>
       </c>
-      <c r="M39" s="30"/>
-      <c r="N39" s="31"/>
+      <c r="M39" s="44"/>
+      <c r="N39" s="48"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="26"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="28"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="24"/>
       <c r="D40" s="25"/>
       <c r="E40" s="25"/>
       <c r="F40" s="3" t="s">
@@ -9181,17 +9181,17 @@
       <c r="I40" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="M40" s="30"/>
-      <c r="N40" s="31"/>
+      <c r="M40" s="44"/>
+      <c r="N40" s="48"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" s="26">
+      <c r="A41" s="22">
         <v>11</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="24" t="s">
         <v>42</v>
       </c>
       <c r="D41" s="25" t="s">
@@ -9212,17 +9212,17 @@
       <c r="I41" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="M41" s="22" t="s">
+      <c r="M41" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="N41" s="23">
+      <c r="N41" s="46">
         <v>45142</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="66" x14ac:dyDescent="0.3">
-      <c r="A42" s="26"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="28"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="24"/>
       <c r="D42" s="25"/>
       <c r="E42" s="25"/>
       <c r="F42" s="3" t="s">
@@ -9243,13 +9243,13 @@
       <c r="L42" t="s">
         <v>58</v>
       </c>
-      <c r="M42" s="22"/>
-      <c r="N42" s="23"/>
+      <c r="M42" s="45"/>
+      <c r="N42" s="46"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" s="26"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="28"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="24"/>
       <c r="D43" s="25"/>
       <c r="E43" s="25"/>
       <c r="F43" s="3" t="s">
@@ -9270,13 +9270,13 @@
       <c r="L43" t="s">
         <v>58</v>
       </c>
-      <c r="M43" s="22"/>
-      <c r="N43" s="23"/>
+      <c r="M43" s="45"/>
+      <c r="N43" s="46"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A44" s="26"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="28"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="24"/>
       <c r="D44" s="25"/>
       <c r="E44" s="25"/>
       <c r="F44" s="3" t="s">
@@ -9297,13 +9297,13 @@
       <c r="L44" t="s">
         <v>58</v>
       </c>
-      <c r="M44" s="22"/>
-      <c r="N44" s="23"/>
+      <c r="M44" s="45"/>
+      <c r="N44" s="46"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A45" s="26"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="28"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="24"/>
       <c r="D45" s="25"/>
       <c r="E45" s="25"/>
       <c r="F45" s="3" t="s">
@@ -9318,13 +9318,13 @@
       <c r="I45" t="s">
         <v>98</v>
       </c>
-      <c r="M45" s="22"/>
-      <c r="N45" s="23"/>
+      <c r="M45" s="45"/>
+      <c r="N45" s="46"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A46" s="26"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="28"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="24"/>
       <c r="D46" s="25"/>
       <c r="E46" s="25"/>
       <c r="F46" s="3" t="s">
@@ -9345,13 +9345,13 @@
       <c r="L46" t="s">
         <v>58</v>
       </c>
-      <c r="M46" s="22"/>
-      <c r="N46" s="23"/>
+      <c r="M46" s="45"/>
+      <c r="N46" s="46"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A47" s="26"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="28"/>
+      <c r="A47" s="22"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="24"/>
       <c r="D47" s="25"/>
       <c r="E47" s="25"/>
       <c r="F47" s="3" t="s">
@@ -9366,17 +9366,17 @@
       <c r="I47" t="s">
         <v>104</v>
       </c>
-      <c r="M47" s="22"/>
-      <c r="N47" s="23"/>
+      <c r="M47" s="45"/>
+      <c r="N47" s="46"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A48" s="26">
+      <c r="A48" s="22">
         <v>12</v>
       </c>
-      <c r="B48" s="27" t="s">
+      <c r="B48" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C48" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D48" s="25" t="s">
@@ -9403,17 +9403,17 @@
       <c r="L48" t="s">
         <v>58</v>
       </c>
-      <c r="M48" s="22" t="s">
+      <c r="M48" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="N48" s="31">
+      <c r="N48" s="48">
         <v>45145</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A49" s="26"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="28"/>
+      <c r="A49" s="22"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="24"/>
       <c r="D49" s="25"/>
       <c r="E49" s="25"/>
       <c r="F49" s="3" t="s">
@@ -9434,13 +9434,13 @@
       <c r="L49" t="s">
         <v>58</v>
       </c>
-      <c r="M49" s="24"/>
-      <c r="N49" s="31"/>
+      <c r="M49" s="47"/>
+      <c r="N49" s="48"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A50" s="26"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="28"/>
+      <c r="A50" s="22"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="24"/>
       <c r="D50" s="25"/>
       <c r="E50" s="25"/>
       <c r="F50" s="3" t="s">
@@ -9461,13 +9461,13 @@
       <c r="L50" t="s">
         <v>58</v>
       </c>
-      <c r="M50" s="24"/>
-      <c r="N50" s="31"/>
+      <c r="M50" s="47"/>
+      <c r="N50" s="48"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A51" s="26"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="28"/>
+      <c r="A51" s="22"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="24"/>
       <c r="D51" s="25"/>
       <c r="E51" s="25"/>
       <c r="F51" s="3" t="s">
@@ -9488,13 +9488,13 @@
       <c r="L51" t="s">
         <v>58</v>
       </c>
-      <c r="M51" s="24"/>
-      <c r="N51" s="31"/>
+      <c r="M51" s="47"/>
+      <c r="N51" s="48"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A52" s="26"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="28"/>
+      <c r="A52" s="22"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="24"/>
       <c r="D52" s="25"/>
       <c r="E52" s="25"/>
       <c r="F52" s="3" t="s">
@@ -9509,13 +9509,13 @@
       <c r="I52" t="s">
         <v>98</v>
       </c>
-      <c r="M52" s="24"/>
-      <c r="N52" s="31"/>
+      <c r="M52" s="47"/>
+      <c r="N52" s="48"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A53" s="26"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="28"/>
+      <c r="A53" s="22"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="24"/>
       <c r="D53" s="25"/>
       <c r="E53" s="25"/>
       <c r="F53" s="3" t="s">
@@ -9536,13 +9536,13 @@
       <c r="L53" t="s">
         <v>62</v>
       </c>
-      <c r="M53" s="24"/>
-      <c r="N53" s="31"/>
+      <c r="M53" s="47"/>
+      <c r="N53" s="48"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A54" s="26"/>
-      <c r="B54" s="27"/>
-      <c r="C54" s="28"/>
+      <c r="A54" s="22"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="24"/>
       <c r="D54" s="25"/>
       <c r="E54" s="25"/>
       <c r="F54" s="3" t="s">
@@ -9557,17 +9557,17 @@
       <c r="I54" t="s">
         <v>104</v>
       </c>
-      <c r="M54" s="24"/>
-      <c r="N54" s="31"/>
+      <c r="M54" s="47"/>
+      <c r="N54" s="48"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A55" s="26">
+      <c r="A55" s="22">
         <v>13</v>
       </c>
-      <c r="B55" s="27" t="s">
+      <c r="B55" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C55" s="28" t="s">
+      <c r="C55" s="24" t="s">
         <v>44</v>
       </c>
       <c r="D55" s="25" t="s">
@@ -9594,17 +9594,17 @@
       <c r="L55" t="s">
         <v>58</v>
       </c>
-      <c r="M55" s="22" t="s">
+      <c r="M55" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="N55" s="23">
+      <c r="N55" s="46">
         <v>45145</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A56" s="26"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="28"/>
+      <c r="A56" s="22"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="24"/>
       <c r="D56" s="25"/>
       <c r="E56" s="25"/>
       <c r="F56" s="3" t="s">
@@ -9625,13 +9625,13 @@
       <c r="L56" t="s">
         <v>58</v>
       </c>
-      <c r="M56" s="22"/>
-      <c r="N56" s="23"/>
+      <c r="M56" s="45"/>
+      <c r="N56" s="46"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A57" s="26"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="28"/>
+      <c r="A57" s="22"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="24"/>
       <c r="D57" s="25"/>
       <c r="E57" s="25"/>
       <c r="F57" s="3" t="s">
@@ -9652,13 +9652,13 @@
       <c r="L57" t="s">
         <v>58</v>
       </c>
-      <c r="M57" s="22"/>
-      <c r="N57" s="23"/>
+      <c r="M57" s="45"/>
+      <c r="N57" s="46"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A58" s="26"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="28"/>
+      <c r="A58" s="22"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="24"/>
       <c r="D58" s="25"/>
       <c r="E58" s="25"/>
       <c r="F58" s="3" t="s">
@@ -9679,13 +9679,13 @@
       <c r="L58" t="s">
         <v>58</v>
       </c>
-      <c r="M58" s="22"/>
-      <c r="N58" s="23"/>
+      <c r="M58" s="45"/>
+      <c r="N58" s="46"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A59" s="26"/>
-      <c r="B59" s="27"/>
-      <c r="C59" s="28"/>
+      <c r="A59" s="22"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="24"/>
       <c r="D59" s="25"/>
       <c r="E59" s="25"/>
       <c r="F59" s="3" t="s">
@@ -9700,13 +9700,13 @@
       <c r="I59" t="s">
         <v>98</v>
       </c>
-      <c r="M59" s="22"/>
-      <c r="N59" s="23"/>
+      <c r="M59" s="45"/>
+      <c r="N59" s="46"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A60" s="26"/>
-      <c r="B60" s="27"/>
-      <c r="C60" s="28"/>
+      <c r="A60" s="22"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="24"/>
       <c r="D60" s="25"/>
       <c r="E60" s="25"/>
       <c r="F60" s="3" t="s">
@@ -9727,13 +9727,13 @@
       <c r="L60" t="s">
         <v>57</v>
       </c>
-      <c r="M60" s="22"/>
-      <c r="N60" s="23"/>
+      <c r="M60" s="45"/>
+      <c r="N60" s="46"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A61" s="26"/>
-      <c r="B61" s="27"/>
-      <c r="C61" s="28"/>
+      <c r="A61" s="22"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="24"/>
       <c r="D61" s="25"/>
       <c r="E61" s="25"/>
       <c r="F61" s="3" t="s">
@@ -9748,17 +9748,17 @@
       <c r="I61" t="s">
         <v>104</v>
       </c>
-      <c r="M61" s="22"/>
-      <c r="N61" s="23"/>
+      <c r="M61" s="45"/>
+      <c r="N61" s="46"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A62" s="26">
+      <c r="A62" s="22">
         <v>14</v>
       </c>
-      <c r="B62" s="27" t="s">
+      <c r="B62" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C62" s="28" t="s">
+      <c r="C62" s="24" t="s">
         <v>45</v>
       </c>
       <c r="D62" s="25" t="s">
@@ -9779,17 +9779,17 @@
       <c r="I62" t="s">
         <v>77</v>
       </c>
-      <c r="M62" s="22" t="s">
+      <c r="M62" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="N62" s="23">
+      <c r="N62" s="46">
         <v>45145</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A63" s="26"/>
-      <c r="B63" s="27"/>
-      <c r="C63" s="28"/>
+      <c r="A63" s="22"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="24"/>
       <c r="D63" s="25"/>
       <c r="E63" s="25"/>
       <c r="F63" s="3" t="s">
@@ -9810,13 +9810,13 @@
       <c r="L63" t="s">
         <v>57</v>
       </c>
-      <c r="M63" s="22"/>
-      <c r="N63" s="23"/>
+      <c r="M63" s="45"/>
+      <c r="N63" s="46"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A64" s="26"/>
-      <c r="B64" s="27"/>
-      <c r="C64" s="28"/>
+      <c r="A64" s="22"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="24"/>
       <c r="D64" s="25"/>
       <c r="E64" s="25"/>
       <c r="F64" s="3" t="s">
@@ -9837,13 +9837,13 @@
       <c r="L64" t="s">
         <v>57</v>
       </c>
-      <c r="M64" s="22"/>
-      <c r="N64" s="23"/>
+      <c r="M64" s="45"/>
+      <c r="N64" s="46"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A65" s="26"/>
-      <c r="B65" s="27"/>
-      <c r="C65" s="28"/>
+      <c r="A65" s="22"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="24"/>
       <c r="D65" s="25"/>
       <c r="E65" s="25"/>
       <c r="F65" s="3" t="s">
@@ -9864,13 +9864,13 @@
       <c r="L65" t="s">
         <v>57</v>
       </c>
-      <c r="M65" s="22"/>
-      <c r="N65" s="23"/>
+      <c r="M65" s="45"/>
+      <c r="N65" s="46"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A66" s="26"/>
-      <c r="B66" s="27"/>
-      <c r="C66" s="28"/>
+      <c r="A66" s="22"/>
+      <c r="B66" s="23"/>
+      <c r="C66" s="24"/>
       <c r="D66" s="25"/>
       <c r="E66" s="25"/>
       <c r="F66" s="3" t="s">
@@ -9891,13 +9891,13 @@
       <c r="L66" t="s">
         <v>57</v>
       </c>
-      <c r="M66" s="22"/>
-      <c r="N66" s="23"/>
+      <c r="M66" s="45"/>
+      <c r="N66" s="46"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A67" s="26"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="28"/>
+      <c r="A67" s="22"/>
+      <c r="B67" s="23"/>
+      <c r="C67" s="24"/>
       <c r="D67" s="25"/>
       <c r="E67" s="25"/>
       <c r="F67" s="3" t="s">
@@ -9912,13 +9912,13 @@
       <c r="I67" t="s">
         <v>102</v>
       </c>
-      <c r="M67" s="22"/>
-      <c r="N67" s="23"/>
+      <c r="M67" s="45"/>
+      <c r="N67" s="46"/>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A68" s="26"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="28"/>
+      <c r="A68" s="22"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="24"/>
       <c r="D68" s="25"/>
       <c r="E68" s="25"/>
       <c r="F68" s="3" t="s">
@@ -9939,17 +9939,17 @@
       <c r="L68" t="s">
         <v>57</v>
       </c>
-      <c r="M68" s="22"/>
-      <c r="N68" s="23"/>
+      <c r="M68" s="45"/>
+      <c r="N68" s="46"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A69" s="26">
+      <c r="A69" s="22">
         <v>14</v>
       </c>
-      <c r="B69" s="27" t="s">
+      <c r="B69" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C69" s="28" t="s">
+      <c r="C69" s="24" t="s">
         <v>46</v>
       </c>
       <c r="D69" s="25" t="s">
@@ -9970,14 +9970,14 @@
       <c r="I69" t="s">
         <v>77</v>
       </c>
-      <c r="M69" s="22" t="s">
+      <c r="M69" s="45" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A70" s="26"/>
-      <c r="B70" s="27"/>
-      <c r="C70" s="28"/>
+      <c r="A70" s="22"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="24"/>
       <c r="D70" s="25"/>
       <c r="E70" s="25"/>
       <c r="F70" s="3" t="s">
@@ -9998,15 +9998,15 @@
       <c r="L70" t="s">
         <v>58</v>
       </c>
-      <c r="M70" s="22"/>
+      <c r="M70" s="45"/>
       <c r="N70" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A71" s="26"/>
-      <c r="B71" s="27"/>
-      <c r="C71" s="28"/>
+      <c r="A71" s="22"/>
+      <c r="B71" s="23"/>
+      <c r="C71" s="24"/>
       <c r="D71" s="25"/>
       <c r="E71" s="25"/>
       <c r="F71" s="3" t="s">
@@ -10027,15 +10027,15 @@
       <c r="L71" t="s">
         <v>58</v>
       </c>
-      <c r="M71" s="22"/>
+      <c r="M71" s="45"/>
       <c r="N71" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A72" s="26"/>
-      <c r="B72" s="27"/>
-      <c r="C72" s="28"/>
+      <c r="A72" s="22"/>
+      <c r="B72" s="23"/>
+      <c r="C72" s="24"/>
       <c r="D72" s="25"/>
       <c r="E72" s="25"/>
       <c r="F72" s="3" t="s">
@@ -10056,15 +10056,15 @@
       <c r="L72" t="s">
         <v>58</v>
       </c>
-      <c r="M72" s="22"/>
+      <c r="M72" s="45"/>
       <c r="N72" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A73" s="26"/>
-      <c r="B73" s="27"/>
-      <c r="C73" s="28"/>
+      <c r="A73" s="22"/>
+      <c r="B73" s="23"/>
+      <c r="C73" s="24"/>
       <c r="D73" s="25"/>
       <c r="E73" s="25"/>
       <c r="F73" s="3" t="s">
@@ -10079,15 +10079,15 @@
       <c r="I73" t="s">
         <v>98</v>
       </c>
-      <c r="M73" s="22"/>
+      <c r="M73" s="45"/>
       <c r="N73" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A74" s="26"/>
-      <c r="B74" s="27"/>
-      <c r="C74" s="28"/>
+      <c r="A74" s="22"/>
+      <c r="B74" s="23"/>
+      <c r="C74" s="24"/>
       <c r="D74" s="25"/>
       <c r="E74" s="25"/>
       <c r="F74" s="3" t="s">
@@ -10108,15 +10108,15 @@
       <c r="L74" t="s">
         <v>58</v>
       </c>
-      <c r="M74" s="22"/>
+      <c r="M74" s="45"/>
       <c r="N74" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A75" s="26"/>
-      <c r="B75" s="27"/>
-      <c r="C75" s="28"/>
+      <c r="A75" s="22"/>
+      <c r="B75" s="23"/>
+      <c r="C75" s="24"/>
       <c r="D75" s="25"/>
       <c r="E75" s="25"/>
       <c r="F75" s="3" t="s">
@@ -10131,19 +10131,19 @@
       <c r="I75" t="s">
         <v>104</v>
       </c>
-      <c r="M75" s="22"/>
+      <c r="M75" s="45"/>
       <c r="N75" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A76" s="26">
+      <c r="A76" s="22">
         <v>16</v>
       </c>
-      <c r="B76" s="27" t="s">
+      <c r="B76" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C76" s="28" t="s">
+      <c r="C76" s="24" t="s">
         <v>47</v>
       </c>
       <c r="D76" s="25" t="s">
@@ -10167,17 +10167,17 @@
       <c r="K76" t="s">
         <v>74</v>
       </c>
-      <c r="M76" s="22" t="s">
+      <c r="M76" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="N76" s="23">
+      <c r="N76" s="46">
         <v>45142</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A77" s="26"/>
-      <c r="B77" s="27"/>
-      <c r="C77" s="28"/>
+      <c r="A77" s="22"/>
+      <c r="B77" s="23"/>
+      <c r="C77" s="24"/>
       <c r="D77" s="25"/>
       <c r="E77" s="25"/>
       <c r="F77" s="3" t="s">
@@ -10195,13 +10195,13 @@
       <c r="K77" t="s">
         <v>74</v>
       </c>
-      <c r="M77" s="22"/>
-      <c r="N77" s="24"/>
+      <c r="M77" s="45"/>
+      <c r="N77" s="47"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A78" s="26"/>
-      <c r="B78" s="27"/>
-      <c r="C78" s="28"/>
+      <c r="A78" s="22"/>
+      <c r="B78" s="23"/>
+      <c r="C78" s="24"/>
       <c r="D78" s="25"/>
       <c r="E78" s="25"/>
       <c r="F78" s="3" t="s">
@@ -10222,13 +10222,13 @@
       <c r="L78" t="s">
         <v>58</v>
       </c>
-      <c r="M78" s="22"/>
-      <c r="N78" s="24"/>
+      <c r="M78" s="45"/>
+      <c r="N78" s="47"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A79" s="26"/>
-      <c r="B79" s="27"/>
-      <c r="C79" s="28"/>
+      <c r="A79" s="22"/>
+      <c r="B79" s="23"/>
+      <c r="C79" s="24"/>
       <c r="D79" s="25"/>
       <c r="E79" s="25"/>
       <c r="F79" s="3" t="s">
@@ -10249,13 +10249,13 @@
       <c r="L79" t="s">
         <v>58</v>
       </c>
-      <c r="M79" s="22"/>
-      <c r="N79" s="24"/>
+      <c r="M79" s="45"/>
+      <c r="N79" s="47"/>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A80" s="26"/>
-      <c r="B80" s="27"/>
-      <c r="C80" s="28"/>
+      <c r="A80" s="22"/>
+      <c r="B80" s="23"/>
+      <c r="C80" s="24"/>
       <c r="D80" s="25"/>
       <c r="E80" s="25"/>
       <c r="F80" s="3" t="s">
@@ -10273,13 +10273,13 @@
       <c r="K80" t="s">
         <v>74</v>
       </c>
-      <c r="M80" s="22"/>
-      <c r="N80" s="24"/>
+      <c r="M80" s="45"/>
+      <c r="N80" s="47"/>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A81" s="26"/>
-      <c r="B81" s="27"/>
-      <c r="C81" s="28"/>
+      <c r="A81" s="22"/>
+      <c r="B81" s="23"/>
+      <c r="C81" s="24"/>
       <c r="D81" s="25"/>
       <c r="E81" s="25"/>
       <c r="F81" s="3" t="s">
@@ -10300,13 +10300,13 @@
       <c r="L81" t="s">
         <v>58</v>
       </c>
-      <c r="M81" s="22"/>
-      <c r="N81" s="24"/>
+      <c r="M81" s="45"/>
+      <c r="N81" s="47"/>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A82" s="26"/>
-      <c r="B82" s="27"/>
-      <c r="C82" s="28"/>
+      <c r="A82" s="22"/>
+      <c r="B82" s="23"/>
+      <c r="C82" s="24"/>
       <c r="D82" s="25"/>
       <c r="E82" s="25"/>
       <c r="F82" s="3" t="s">
@@ -10324,17 +10324,17 @@
       <c r="K82" t="s">
         <v>74</v>
       </c>
-      <c r="M82" s="22"/>
-      <c r="N82" s="24"/>
+      <c r="M82" s="45"/>
+      <c r="N82" s="47"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A83" s="26">
+      <c r="A83" s="22">
         <v>17</v>
       </c>
-      <c r="B83" s="27" t="s">
+      <c r="B83" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C83" s="28" t="s">
+      <c r="C83" s="24" t="s">
         <v>48</v>
       </c>
       <c r="D83" s="25" t="s">
@@ -10358,17 +10358,17 @@
       <c r="K83" t="s">
         <v>74</v>
       </c>
-      <c r="M83" s="22" t="s">
+      <c r="M83" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="N83" s="23">
+      <c r="N83" s="46">
         <v>45142</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A84" s="26"/>
-      <c r="B84" s="27"/>
-      <c r="C84" s="28"/>
+      <c r="A84" s="22"/>
+      <c r="B84" s="23"/>
+      <c r="C84" s="24"/>
       <c r="D84" s="25"/>
       <c r="E84" s="25"/>
       <c r="F84" s="3" t="s">
@@ -10389,13 +10389,13 @@
       <c r="L84" t="s">
         <v>57</v>
       </c>
-      <c r="M84" s="24"/>
-      <c r="N84" s="24"/>
+      <c r="M84" s="47"/>
+      <c r="N84" s="47"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A85" s="26"/>
-      <c r="B85" s="27"/>
-      <c r="C85" s="28"/>
+      <c r="A85" s="22"/>
+      <c r="B85" s="23"/>
+      <c r="C85" s="24"/>
       <c r="D85" s="25"/>
       <c r="E85" s="25"/>
       <c r="F85" s="3" t="s">
@@ -10416,13 +10416,13 @@
       <c r="L85" t="s">
         <v>57</v>
       </c>
-      <c r="M85" s="24"/>
-      <c r="N85" s="24"/>
+      <c r="M85" s="47"/>
+      <c r="N85" s="47"/>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A86" s="26"/>
-      <c r="B86" s="27"/>
-      <c r="C86" s="28"/>
+      <c r="A86" s="22"/>
+      <c r="B86" s="23"/>
+      <c r="C86" s="24"/>
       <c r="D86" s="25"/>
       <c r="E86" s="25"/>
       <c r="F86" s="3" t="s">
@@ -10443,13 +10443,13 @@
       <c r="L86" t="s">
         <v>57</v>
       </c>
-      <c r="M86" s="24"/>
-      <c r="N86" s="24"/>
+      <c r="M86" s="47"/>
+      <c r="N86" s="47"/>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A87" s="26"/>
-      <c r="B87" s="27"/>
-      <c r="C87" s="28"/>
+      <c r="A87" s="22"/>
+      <c r="B87" s="23"/>
+      <c r="C87" s="24"/>
       <c r="D87" s="25"/>
       <c r="E87" s="25"/>
       <c r="F87" s="3" t="s">
@@ -10467,13 +10467,13 @@
       <c r="K87" t="s">
         <v>74</v>
       </c>
-      <c r="M87" s="24"/>
-      <c r="N87" s="24"/>
+      <c r="M87" s="47"/>
+      <c r="N87" s="47"/>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A88" s="26"/>
-      <c r="B88" s="27"/>
-      <c r="C88" s="28"/>
+      <c r="A88" s="22"/>
+      <c r="B88" s="23"/>
+      <c r="C88" s="24"/>
       <c r="D88" s="25"/>
       <c r="E88" s="25"/>
       <c r="F88" s="3" t="s">
@@ -10494,13 +10494,13 @@
       <c r="L88" t="s">
         <v>57</v>
       </c>
-      <c r="M88" s="24"/>
-      <c r="N88" s="24"/>
+      <c r="M88" s="47"/>
+      <c r="N88" s="47"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A89" s="26"/>
-      <c r="B89" s="27"/>
-      <c r="C89" s="28"/>
+      <c r="A89" s="22"/>
+      <c r="B89" s="23"/>
+      <c r="C89" s="24"/>
       <c r="D89" s="25"/>
       <c r="E89" s="25"/>
       <c r="F89" s="3" t="s">
@@ -10515,17 +10515,17 @@
       <c r="I89" t="s">
         <v>104</v>
       </c>
-      <c r="M89" s="24"/>
-      <c r="N89" s="24"/>
+      <c r="M89" s="47"/>
+      <c r="N89" s="47"/>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A90" s="26">
+      <c r="A90" s="22">
         <v>18</v>
       </c>
-      <c r="B90" s="27" t="s">
+      <c r="B90" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C90" s="28" t="s">
+      <c r="C90" s="24" t="s">
         <v>49</v>
       </c>
       <c r="D90" s="25" t="s">
@@ -10552,17 +10552,17 @@
       <c r="L90" t="s">
         <v>57</v>
       </c>
-      <c r="M90" s="22" t="s">
+      <c r="M90" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="N90" s="23">
+      <c r="N90" s="46">
         <v>45145</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A91" s="26"/>
-      <c r="B91" s="27"/>
-      <c r="C91" s="28"/>
+      <c r="A91" s="22"/>
+      <c r="B91" s="23"/>
+      <c r="C91" s="24"/>
       <c r="D91" s="25"/>
       <c r="E91" s="25"/>
       <c r="F91" s="3" t="s">
@@ -10583,13 +10583,13 @@
       <c r="L91" t="s">
         <v>57</v>
       </c>
-      <c r="M91" s="22"/>
-      <c r="N91" s="23"/>
+      <c r="M91" s="45"/>
+      <c r="N91" s="46"/>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A92" s="26"/>
-      <c r="B92" s="27"/>
-      <c r="C92" s="28"/>
+      <c r="A92" s="22"/>
+      <c r="B92" s="23"/>
+      <c r="C92" s="24"/>
       <c r="D92" s="25"/>
       <c r="E92" s="25"/>
       <c r="F92" s="3" t="s">
@@ -10610,13 +10610,13 @@
       <c r="L92" t="s">
         <v>57</v>
       </c>
-      <c r="M92" s="22"/>
-      <c r="N92" s="23"/>
+      <c r="M92" s="45"/>
+      <c r="N92" s="46"/>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A93" s="26"/>
-      <c r="B93" s="27"/>
-      <c r="C93" s="28"/>
+      <c r="A93" s="22"/>
+      <c r="B93" s="23"/>
+      <c r="C93" s="24"/>
       <c r="D93" s="25"/>
       <c r="E93" s="25"/>
       <c r="F93" s="3" t="s">
@@ -10637,13 +10637,13 @@
       <c r="L93" t="s">
         <v>57</v>
       </c>
-      <c r="M93" s="22"/>
-      <c r="N93" s="23"/>
+      <c r="M93" s="45"/>
+      <c r="N93" s="46"/>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A94" s="26"/>
-      <c r="B94" s="27"/>
-      <c r="C94" s="28"/>
+      <c r="A94" s="22"/>
+      <c r="B94" s="23"/>
+      <c r="C94" s="24"/>
       <c r="D94" s="25"/>
       <c r="E94" s="25"/>
       <c r="F94" s="3" t="s">
@@ -10661,13 +10661,13 @@
       <c r="K94" t="s">
         <v>74</v>
       </c>
-      <c r="M94" s="22"/>
-      <c r="N94" s="23"/>
+      <c r="M94" s="45"/>
+      <c r="N94" s="46"/>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A95" s="26"/>
-      <c r="B95" s="27"/>
-      <c r="C95" s="28"/>
+      <c r="A95" s="22"/>
+      <c r="B95" s="23"/>
+      <c r="C95" s="24"/>
       <c r="D95" s="25"/>
       <c r="E95" s="25"/>
       <c r="F95" s="3" t="s">
@@ -10688,13 +10688,13 @@
       <c r="L95" t="s">
         <v>57</v>
       </c>
-      <c r="M95" s="22"/>
-      <c r="N95" s="23"/>
+      <c r="M95" s="45"/>
+      <c r="N95" s="46"/>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A96" s="26"/>
-      <c r="B96" s="27"/>
-      <c r="C96" s="28"/>
+      <c r="A96" s="22"/>
+      <c r="B96" s="23"/>
+      <c r="C96" s="24"/>
       <c r="D96" s="25"/>
       <c r="E96" s="25"/>
       <c r="F96" s="3" t="s">
@@ -10709,17 +10709,17 @@
       <c r="I96" t="s">
         <v>104</v>
       </c>
-      <c r="M96" s="22"/>
-      <c r="N96" s="23"/>
+      <c r="M96" s="45"/>
+      <c r="N96" s="46"/>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A97" s="26">
+      <c r="A97" s="22">
         <v>19</v>
       </c>
-      <c r="B97" s="27" t="s">
+      <c r="B97" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C97" s="28" t="s">
+      <c r="C97" s="24" t="s">
         <v>50</v>
       </c>
       <c r="D97" s="25" t="s">
@@ -10746,17 +10746,17 @@
       <c r="L97" t="s">
         <v>58</v>
       </c>
-      <c r="M97" s="22" t="s">
+      <c r="M97" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="N97" s="23">
+      <c r="N97" s="46">
         <v>45145</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A98" s="26"/>
-      <c r="B98" s="27"/>
-      <c r="C98" s="28"/>
+      <c r="A98" s="22"/>
+      <c r="B98" s="23"/>
+      <c r="C98" s="24"/>
       <c r="D98" s="25"/>
       <c r="E98" s="25"/>
       <c r="F98" s="3" t="s">
@@ -10777,13 +10777,13 @@
       <c r="L98" t="s">
         <v>58</v>
       </c>
-      <c r="M98" s="22"/>
-      <c r="N98" s="23"/>
+      <c r="M98" s="45"/>
+      <c r="N98" s="46"/>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A99" s="26"/>
-      <c r="B99" s="27"/>
-      <c r="C99" s="28"/>
+      <c r="A99" s="22"/>
+      <c r="B99" s="23"/>
+      <c r="C99" s="24"/>
       <c r="D99" s="25"/>
       <c r="E99" s="25"/>
       <c r="F99" s="3" t="s">
@@ -10804,13 +10804,13 @@
       <c r="L99" t="s">
         <v>58</v>
       </c>
-      <c r="M99" s="22"/>
-      <c r="N99" s="23"/>
+      <c r="M99" s="45"/>
+      <c r="N99" s="46"/>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A100" s="26"/>
-      <c r="B100" s="27"/>
-      <c r="C100" s="28"/>
+      <c r="A100" s="22"/>
+      <c r="B100" s="23"/>
+      <c r="C100" s="24"/>
       <c r="D100" s="25"/>
       <c r="E100" s="25"/>
       <c r="F100" s="3" t="s">
@@ -10831,13 +10831,13 @@
       <c r="L100" t="s">
         <v>58</v>
       </c>
-      <c r="M100" s="22"/>
-      <c r="N100" s="23"/>
+      <c r="M100" s="45"/>
+      <c r="N100" s="46"/>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A101" s="26"/>
-      <c r="B101" s="27"/>
-      <c r="C101" s="28"/>
+      <c r="A101" s="22"/>
+      <c r="B101" s="23"/>
+      <c r="C101" s="24"/>
       <c r="D101" s="25"/>
       <c r="E101" s="25"/>
       <c r="F101" s="3" t="s">
@@ -10855,13 +10855,13 @@
       <c r="K101" t="s">
         <v>74</v>
       </c>
-      <c r="M101" s="22"/>
-      <c r="N101" s="23"/>
+      <c r="M101" s="45"/>
+      <c r="N101" s="46"/>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A102" s="26"/>
-      <c r="B102" s="27"/>
-      <c r="C102" s="28"/>
+      <c r="A102" s="22"/>
+      <c r="B102" s="23"/>
+      <c r="C102" s="24"/>
       <c r="D102" s="25"/>
       <c r="E102" s="25"/>
       <c r="F102" s="3" t="s">
@@ -10882,13 +10882,13 @@
       <c r="L102" t="s">
         <v>58</v>
       </c>
-      <c r="M102" s="22"/>
-      <c r="N102" s="23"/>
+      <c r="M102" s="45"/>
+      <c r="N102" s="46"/>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A103" s="26"/>
-      <c r="B103" s="27"/>
-      <c r="C103" s="28"/>
+      <c r="A103" s="22"/>
+      <c r="B103" s="23"/>
+      <c r="C103" s="24"/>
       <c r="D103" s="25"/>
       <c r="E103" s="25"/>
       <c r="F103" s="3" t="s">
@@ -10903,17 +10903,17 @@
       <c r="I103" t="s">
         <v>104</v>
       </c>
-      <c r="M103" s="22"/>
-      <c r="N103" s="23"/>
+      <c r="M103" s="45"/>
+      <c r="N103" s="46"/>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A104" s="26">
+      <c r="A104" s="22">
         <v>29</v>
       </c>
-      <c r="B104" s="27" t="s">
+      <c r="B104" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C104" s="28" t="s">
+      <c r="C104" s="24" t="s">
         <v>51</v>
       </c>
       <c r="D104" s="25" t="s">
@@ -10934,7 +10934,7 @@
       <c r="K104" t="s">
         <v>74</v>
       </c>
-      <c r="M104" s="22" t="s">
+      <c r="M104" s="45" t="s">
         <v>115</v>
       </c>
       <c r="N104" s="1">
@@ -10942,9 +10942,9 @@
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A105" s="26"/>
-      <c r="B105" s="27"/>
-      <c r="C105" s="28"/>
+      <c r="A105" s="22"/>
+      <c r="B105" s="23"/>
+      <c r="C105" s="24"/>
       <c r="D105" s="25"/>
       <c r="E105" s="25"/>
       <c r="F105" s="3" t="s">
@@ -10965,15 +10965,15 @@
       <c r="L105" t="s">
         <v>58</v>
       </c>
-      <c r="M105" s="22"/>
+      <c r="M105" s="45"/>
       <c r="N105" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A106" s="26"/>
-      <c r="B106" s="27"/>
-      <c r="C106" s="28"/>
+      <c r="A106" s="22"/>
+      <c r="B106" s="23"/>
+      <c r="C106" s="24"/>
       <c r="D106" s="25"/>
       <c r="E106" s="25"/>
       <c r="F106" s="3" t="s">
@@ -10994,15 +10994,15 @@
       <c r="L106" t="s">
         <v>58</v>
       </c>
-      <c r="M106" s="22"/>
+      <c r="M106" s="45"/>
       <c r="N106" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A107" s="26"/>
-      <c r="B107" s="27"/>
-      <c r="C107" s="28"/>
+      <c r="A107" s="22"/>
+      <c r="B107" s="23"/>
+      <c r="C107" s="24"/>
       <c r="D107" s="25"/>
       <c r="E107" s="25"/>
       <c r="F107" s="3" t="s">
@@ -11023,15 +11023,15 @@
       <c r="L107" t="s">
         <v>58</v>
       </c>
-      <c r="M107" s="22"/>
+      <c r="M107" s="45"/>
       <c r="N107" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A108" s="26"/>
-      <c r="B108" s="27"/>
-      <c r="C108" s="28"/>
+      <c r="A108" s="22"/>
+      <c r="B108" s="23"/>
+      <c r="C108" s="24"/>
       <c r="D108" s="25"/>
       <c r="E108" s="25"/>
       <c r="F108" s="3" t="s">
@@ -11049,15 +11049,15 @@
       <c r="L108" t="s">
         <v>57</v>
       </c>
-      <c r="M108" s="22"/>
+      <c r="M108" s="45"/>
       <c r="N108" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A109" s="26"/>
-      <c r="B109" s="27"/>
-      <c r="C109" s="28"/>
+      <c r="A109" s="22"/>
+      <c r="B109" s="23"/>
+      <c r="C109" s="24"/>
       <c r="D109" s="25"/>
       <c r="E109" s="25"/>
       <c r="F109" s="3" t="s">
@@ -11078,15 +11078,15 @@
       <c r="L109" t="s">
         <v>58</v>
       </c>
-      <c r="M109" s="22"/>
+      <c r="M109" s="45"/>
       <c r="N109" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A110" s="26"/>
-      <c r="B110" s="27"/>
-      <c r="C110" s="28"/>
+      <c r="A110" s="22"/>
+      <c r="B110" s="23"/>
+      <c r="C110" s="24"/>
       <c r="D110" s="25"/>
       <c r="E110" s="25"/>
       <c r="F110" s="3" t="s">
@@ -11101,19 +11101,19 @@
       <c r="I110" t="s">
         <v>104</v>
       </c>
-      <c r="M110" s="22"/>
+      <c r="M110" s="45"/>
       <c r="N110" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A111" s="26">
+      <c r="A111" s="22">
         <v>29</v>
       </c>
-      <c r="B111" s="27" t="s">
+      <c r="B111" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C111" s="28" t="s">
+      <c r="C111" s="24" t="s">
         <v>121</v>
       </c>
       <c r="D111" s="25" t="s">
@@ -11137,7 +11137,7 @@
       <c r="L111" t="s">
         <v>57</v>
       </c>
-      <c r="M111" s="29" t="s">
+      <c r="M111" s="43" t="s">
         <v>132</v>
       </c>
       <c r="N111" s="1">
@@ -11145,9 +11145,9 @@
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A112" s="26"/>
-      <c r="B112" s="27"/>
-      <c r="C112" s="28"/>
+      <c r="A112" s="22"/>
+      <c r="B112" s="23"/>
+      <c r="C112" s="24"/>
       <c r="D112" s="25"/>
       <c r="E112" s="25"/>
       <c r="F112" s="3" t="s">
@@ -11168,15 +11168,15 @@
       <c r="L112" t="s">
         <v>57</v>
       </c>
-      <c r="M112" s="30"/>
+      <c r="M112" s="44"/>
       <c r="N112" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A113" s="26"/>
-      <c r="B113" s="27"/>
-      <c r="C113" s="28"/>
+      <c r="A113" s="22"/>
+      <c r="B113" s="23"/>
+      <c r="C113" s="24"/>
       <c r="D113" s="25"/>
       <c r="E113" s="25"/>
       <c r="F113" s="3" t="s">
@@ -11197,15 +11197,15 @@
       <c r="L113" t="s">
         <v>57</v>
       </c>
-      <c r="M113" s="30"/>
+      <c r="M113" s="44"/>
       <c r="N113" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A114" s="26"/>
-      <c r="B114" s="27"/>
-      <c r="C114" s="28"/>
+      <c r="A114" s="22"/>
+      <c r="B114" s="23"/>
+      <c r="C114" s="24"/>
       <c r="D114" s="25"/>
       <c r="E114" s="25"/>
       <c r="F114" s="3" t="s">
@@ -11226,15 +11226,15 @@
       <c r="L114" t="s">
         <v>57</v>
       </c>
-      <c r="M114" s="30"/>
+      <c r="M114" s="44"/>
       <c r="N114" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A115" s="26"/>
-      <c r="B115" s="27"/>
-      <c r="C115" s="28"/>
+      <c r="A115" s="22"/>
+      <c r="B115" s="23"/>
+      <c r="C115" s="24"/>
       <c r="D115" s="25"/>
       <c r="E115" s="25"/>
       <c r="F115" s="3" t="s">
@@ -11252,15 +11252,15 @@
       <c r="L115" t="s">
         <v>57</v>
       </c>
-      <c r="M115" s="30"/>
+      <c r="M115" s="44"/>
       <c r="N115" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A116" s="26"/>
-      <c r="B116" s="27"/>
-      <c r="C116" s="28"/>
+      <c r="A116" s="22"/>
+      <c r="B116" s="23"/>
+      <c r="C116" s="24"/>
       <c r="D116" s="25"/>
       <c r="E116" s="25"/>
       <c r="F116" s="3" t="s">
@@ -11281,15 +11281,15 @@
       <c r="L116" t="s">
         <v>57</v>
       </c>
-      <c r="M116" s="30"/>
+      <c r="M116" s="44"/>
       <c r="N116" s="1">
         <v>45142</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A117" s="26"/>
-      <c r="B117" s="27"/>
-      <c r="C117" s="28"/>
+      <c r="A117" s="22"/>
+      <c r="B117" s="23"/>
+      <c r="C117" s="24"/>
       <c r="D117" s="25"/>
       <c r="E117" s="25"/>
       <c r="F117" s="3" t="s">
@@ -11304,7 +11304,7 @@
       <c r="I117" t="s">
         <v>104</v>
       </c>
-      <c r="M117" s="30"/>
+      <c r="M117" s="44"/>
       <c r="N117" s="1">
         <v>45142</v>
       </c>
@@ -11312,56 +11312,41 @@
   </sheetData>
   <autoFilter ref="G1:G117"/>
   <mergeCells count="109">
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B13:B19"/>
-    <mergeCell ref="C13:C19"/>
-    <mergeCell ref="D13:D19"/>
-    <mergeCell ref="E13:E19"/>
-    <mergeCell ref="A1:N2"/>
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="E3:F4"/>
-    <mergeCell ref="G3:N4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:B26"/>
-    <mergeCell ref="C20:C26"/>
-    <mergeCell ref="D20:D26"/>
-    <mergeCell ref="E20:E26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:B33"/>
-    <mergeCell ref="C27:C33"/>
-    <mergeCell ref="D27:D33"/>
-    <mergeCell ref="E27:E33"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="B34:B40"/>
-    <mergeCell ref="C34:C40"/>
-    <mergeCell ref="D34:D40"/>
-    <mergeCell ref="E34:E40"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="B48:B54"/>
-    <mergeCell ref="C48:C54"/>
-    <mergeCell ref="D48:D54"/>
-    <mergeCell ref="E48:E54"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="B41:B47"/>
-    <mergeCell ref="C41:C47"/>
-    <mergeCell ref="D41:D47"/>
-    <mergeCell ref="E41:E47"/>
-    <mergeCell ref="C69:C75"/>
-    <mergeCell ref="D69:D75"/>
-    <mergeCell ref="E69:E75"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:B82"/>
-    <mergeCell ref="C76:C82"/>
-    <mergeCell ref="D76:D82"/>
-    <mergeCell ref="E76:E82"/>
-    <mergeCell ref="A83:A89"/>
-    <mergeCell ref="B83:B89"/>
-    <mergeCell ref="C83:C89"/>
-    <mergeCell ref="D83:D89"/>
-    <mergeCell ref="E83:E89"/>
+    <mergeCell ref="M90:M96"/>
+    <mergeCell ref="N90:N96"/>
+    <mergeCell ref="M97:M103"/>
+    <mergeCell ref="N97:N103"/>
+    <mergeCell ref="M104:M110"/>
+    <mergeCell ref="N55:N61"/>
+    <mergeCell ref="M62:M68"/>
+    <mergeCell ref="N62:N68"/>
+    <mergeCell ref="M69:M75"/>
+    <mergeCell ref="M83:M89"/>
+    <mergeCell ref="N83:N89"/>
+    <mergeCell ref="D111:D117"/>
+    <mergeCell ref="E111:E117"/>
+    <mergeCell ref="A111:A117"/>
+    <mergeCell ref="B111:B117"/>
+    <mergeCell ref="C111:C117"/>
+    <mergeCell ref="M111:M117"/>
+    <mergeCell ref="M76:M82"/>
+    <mergeCell ref="N76:N82"/>
+    <mergeCell ref="M13:M19"/>
+    <mergeCell ref="N13:N19"/>
+    <mergeCell ref="M20:M26"/>
+    <mergeCell ref="N20:N26"/>
+    <mergeCell ref="M27:M33"/>
+    <mergeCell ref="N27:N33"/>
+    <mergeCell ref="M34:M40"/>
+    <mergeCell ref="N34:N40"/>
+    <mergeCell ref="M41:M47"/>
+    <mergeCell ref="N41:N47"/>
+    <mergeCell ref="M48:M54"/>
+    <mergeCell ref="N48:N54"/>
+    <mergeCell ref="M55:M61"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="B104:B110"/>
+    <mergeCell ref="C104:C110"/>
     <mergeCell ref="D104:D110"/>
     <mergeCell ref="E104:E110"/>
     <mergeCell ref="A97:A103"/>
@@ -11386,41 +11371,56 @@
     <mergeCell ref="E90:E96"/>
     <mergeCell ref="A69:A75"/>
     <mergeCell ref="B69:B75"/>
-    <mergeCell ref="D111:D117"/>
-    <mergeCell ref="E111:E117"/>
-    <mergeCell ref="A111:A117"/>
-    <mergeCell ref="B111:B117"/>
-    <mergeCell ref="C111:C117"/>
-    <mergeCell ref="M111:M117"/>
-    <mergeCell ref="M76:M82"/>
-    <mergeCell ref="N76:N82"/>
-    <mergeCell ref="M13:M19"/>
-    <mergeCell ref="N13:N19"/>
-    <mergeCell ref="M20:M26"/>
-    <mergeCell ref="N20:N26"/>
-    <mergeCell ref="M27:M33"/>
-    <mergeCell ref="N27:N33"/>
-    <mergeCell ref="M34:M40"/>
-    <mergeCell ref="N34:N40"/>
-    <mergeCell ref="M41:M47"/>
-    <mergeCell ref="N41:N47"/>
-    <mergeCell ref="M48:M54"/>
-    <mergeCell ref="N48:N54"/>
-    <mergeCell ref="M55:M61"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="B104:B110"/>
-    <mergeCell ref="C104:C110"/>
-    <mergeCell ref="M90:M96"/>
-    <mergeCell ref="N90:N96"/>
-    <mergeCell ref="M97:M103"/>
-    <mergeCell ref="N97:N103"/>
-    <mergeCell ref="M104:M110"/>
-    <mergeCell ref="N55:N61"/>
-    <mergeCell ref="M62:M68"/>
-    <mergeCell ref="N62:N68"/>
-    <mergeCell ref="M69:M75"/>
-    <mergeCell ref="M83:M89"/>
-    <mergeCell ref="N83:N89"/>
+    <mergeCell ref="C69:C75"/>
+    <mergeCell ref="D69:D75"/>
+    <mergeCell ref="E69:E75"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:B82"/>
+    <mergeCell ref="C76:C82"/>
+    <mergeCell ref="D76:D82"/>
+    <mergeCell ref="E76:E82"/>
+    <mergeCell ref="A83:A89"/>
+    <mergeCell ref="B83:B89"/>
+    <mergeCell ref="C83:C89"/>
+    <mergeCell ref="D83:D89"/>
+    <mergeCell ref="E83:E89"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="C34:C40"/>
+    <mergeCell ref="D34:D40"/>
+    <mergeCell ref="E34:E40"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="B48:B54"/>
+    <mergeCell ref="C48:C54"/>
+    <mergeCell ref="D48:D54"/>
+    <mergeCell ref="E48:E54"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="C41:C47"/>
+    <mergeCell ref="D41:D47"/>
+    <mergeCell ref="E41:E47"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:B26"/>
+    <mergeCell ref="C20:C26"/>
+    <mergeCell ref="D20:D26"/>
+    <mergeCell ref="E20:E26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="B27:B33"/>
+    <mergeCell ref="C27:C33"/>
+    <mergeCell ref="D27:D33"/>
+    <mergeCell ref="E27:E33"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="C13:C19"/>
+    <mergeCell ref="D13:D19"/>
+    <mergeCell ref="E13:E19"/>
+    <mergeCell ref="A1:N2"/>
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="G3:N4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:N5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M11" r:id="rId1"/>

</xml_diff>